<commit_message>
Add new monthly series
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_mensual.xlsx
+++ b/etl/data/input/Datos_carga_mensual.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Paro" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
   <si>
     <t xml:space="preserve">Año</t>
   </si>
@@ -344,6 +344,9 @@
   <si>
     <t xml:space="preserve">Beneficiarios prestaciones por desempleos España. Tendencia</t>
   </si>
+  <si>
+    <t xml:space="preserve">Beneficiarios prestaciones por desempleos Cantabria</t>
+  </si>
 </sst>
 </file>
 
@@ -4162,7 +4165,7 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
     </sheetView>
   </sheetViews>
@@ -5778,8 +5781,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6590,8 +6593,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7407,8 +7410,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8216,8 +8219,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8240,8 +8243,8 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
-        <v>0</v>
+      <c r="C1" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
Minor fixes in metadata
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_mensual.xlsx
+++ b/etl/data/input/Datos_carga_mensual.xlsx
@@ -352,12 +352,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="169" formatCode="0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -432,7 +433,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -458,6 +459,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8217,10 +8222,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8262,14 +8267,14 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>2018</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="7" t="n">
         <v>18236</v>
       </c>
       <c r="D2" s="3" t="n">
@@ -8278,8 +8283,8 @@
       <c r="E2" s="3" t="n">
         <v>-4.77331792996356</v>
       </c>
-      <c r="F2" s="6" t="n">
-        <v>1596963.02</v>
+      <c r="F2" s="7" t="n">
+        <v>1596963</v>
       </c>
       <c r="G2" s="3" t="n">
         <v>-0.754865902114654</v>
@@ -8288,7 +8293,7 @@
         <v>-2.28476112892554</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <f aca="false">A2</f>
         <v>2018</v>
@@ -8296,7 +8301,7 @@
       <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="7" t="n">
         <v>18656</v>
       </c>
       <c r="D3" s="3" t="n">
@@ -8305,8 +8310,8 @@
       <c r="E3" s="3" t="n">
         <v>-4.18358357594205</v>
       </c>
-      <c r="F3" s="6" t="n">
-        <v>1547593.05</v>
+      <c r="F3" s="7" t="n">
+        <v>1547593</v>
       </c>
       <c r="G3" s="3" t="n">
         <v>-1.18605551478654</v>
@@ -8315,7 +8320,7 @@
         <v>-1.75574327209982</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <f aca="false">A3</f>
         <v>2018</v>
@@ -8323,7 +8328,7 @@
       <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="7" t="n">
         <v>16737</v>
       </c>
       <c r="D4" s="3" t="n">
@@ -8332,8 +8337,8 @@
       <c r="E4" s="3" t="n">
         <v>-3.57928323797541</v>
       </c>
-      <c r="F4" s="6" t="n">
-        <v>1469617.4</v>
+      <c r="F4" s="7" t="n">
+        <v>1469617</v>
       </c>
       <c r="G4" s="3" t="n">
         <v>-1.99895949147345</v>
@@ -8342,7 +8347,7 @@
         <v>-1.21712365699383</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <f aca="false">A4</f>
         <v>2018</v>
@@ -8350,7 +8355,7 @@
       <c r="B5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="7" t="n">
         <v>15548</v>
       </c>
       <c r="D5" s="3" t="n">
@@ -8359,8 +8364,8 @@
       <c r="E5" s="3" t="n">
         <v>-2.95978566834487</v>
       </c>
-      <c r="F5" s="6" t="n">
-        <v>1399495.46</v>
+      <c r="F5" s="7" t="n">
+        <v>1399495</v>
       </c>
       <c r="G5" s="3" t="n">
         <v>0.767232460491862</v>
@@ -8369,7 +8374,7 @@
         <v>-0.668674206841622</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <f aca="false">A5</f>
         <v>2018</v>
@@ -8377,7 +8382,7 @@
       <c r="B6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="7" t="n">
         <v>14486</v>
       </c>
       <c r="D6" s="3" t="n">
@@ -8386,8 +8391,8 @@
       <c r="E6" s="3" t="n">
         <v>-2.32451383577348</v>
       </c>
-      <c r="F6" s="6" t="n">
-        <v>1343721.94</v>
+      <c r="F6" s="7" t="n">
+        <v>1343722</v>
       </c>
       <c r="G6" s="3" t="n">
         <v>-0.882903009975644</v>
@@ -8396,7 +8401,7 @@
         <v>-0.110221139032413</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <f aca="false">A6</f>
         <v>2018</v>
@@ -8404,7 +8409,7 @@
       <c r="B7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="C7" s="7" t="n">
         <v>13710</v>
       </c>
       <c r="D7" s="3" t="n">
@@ -8413,8 +8418,8 @@
       <c r="E7" s="3" t="n">
         <v>-1.67293822565875</v>
       </c>
-      <c r="F7" s="6" t="n">
-        <v>1318885.39</v>
+      <c r="F7" s="7" t="n">
+        <v>1318885</v>
       </c>
       <c r="G7" s="3" t="n">
         <v>-0.4747082257618</v>
@@ -8423,7 +8428,7 @@
         <v>0.45850904478536</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <f aca="false">A7</f>
         <v>2018</v>
@@ -8431,7 +8436,7 @@
       <c r="B8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="7" t="n">
         <v>13299</v>
       </c>
       <c r="D8" s="3" t="n">
@@ -8440,8 +8445,8 @@
       <c r="E8" s="3" t="n">
         <v>-1.00483014582102</v>
       </c>
-      <c r="F8" s="6" t="n">
-        <v>1400991.06</v>
+      <c r="F8" s="7" t="n">
+        <v>1400991</v>
       </c>
       <c r="G8" s="3" t="n">
         <v>-1.01439344688211</v>
@@ -8450,7 +8455,7 @@
         <v>1.0377361845</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <f aca="false">A8</f>
         <v>2018</v>
@@ -8458,7 +8463,7 @@
       <c r="B9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="7" t="n">
         <v>13990</v>
       </c>
       <c r="D9" s="3" t="n">
@@ -8467,8 +8472,8 @@
       <c r="E9" s="3" t="n">
         <v>-0.320141938206918</v>
       </c>
-      <c r="F9" s="6" t="n">
-        <v>1503242.36</v>
+      <c r="F9" s="7" t="n">
+        <v>1503242</v>
       </c>
       <c r="G9" s="3" t="n">
         <v>-0.42131355212629</v>
@@ -8477,7 +8482,7 @@
         <v>1.62761531324492</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <f aca="false">A9</f>
         <v>2018</v>
@@ -8485,7 +8490,7 @@
       <c r="B10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="7" t="n">
         <v>13375</v>
       </c>
       <c r="D10" s="3" t="n">
@@ -8494,8 +8499,8 @@
       <c r="E10" s="3" t="n">
         <v>0.380948358746267</v>
       </c>
-      <c r="F10" s="6" t="n">
-        <v>1425852.78</v>
+      <c r="F10" s="7" t="n">
+        <v>1425853</v>
       </c>
       <c r="G10" s="3" t="n">
         <v>0.79841435216752</v>
@@ -8504,7 +8509,7 @@
         <v>2.22815895515135</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <f aca="false">A10</f>
         <v>2018</v>
@@ -8512,7 +8517,7 @@
       <c r="B11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="7" t="n">
         <v>14433</v>
       </c>
       <c r="D11" s="3" t="n">
@@ -8521,8 +8526,8 @@
       <c r="E11" s="3" t="n">
         <v>1.09814057667287</v>
       </c>
-      <c r="F11" s="6" t="n">
-        <v>1431092.16</v>
+      <c r="F11" s="7" t="n">
+        <v>1431092</v>
       </c>
       <c r="G11" s="3" t="n">
         <v>0.803239493368912</v>
@@ -8531,7 +8536,7 @@
         <v>2.83923734762374</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <f aca="false">A11</f>
         <v>2018</v>
@@ -8539,7 +8544,7 @@
       <c r="B12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C12" s="6" t="n">
+      <c r="C12" s="7" t="n">
         <v>15558</v>
       </c>
       <c r="D12" s="3" t="n">
@@ -8548,8 +8553,8 @@
       <c r="E12" s="3" t="n">
         <v>1.83082042035451</v>
       </c>
-      <c r="F12" s="6" t="n">
-        <v>1507438.81</v>
+      <c r="F12" s="7" t="n">
+        <v>1507439</v>
       </c>
       <c r="G12" s="3" t="n">
         <v>2.05123592955896</v>
@@ -8558,7 +8563,7 @@
         <v>3.46062144024691</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <f aca="false">A12</f>
         <v>2018</v>
@@ -8566,7 +8571,7 @@
       <c r="B13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="C13" s="6" t="n">
+      <c r="C13" s="7" t="n">
         <v>16407</v>
       </c>
       <c r="D13" s="3" t="n">
@@ -8575,8 +8580,8 @@
       <c r="E13" s="3" t="n">
         <v>2.57821414219162</v>
       </c>
-      <c r="F13" s="6" t="n">
-        <v>1524413.83</v>
+      <c r="F13" s="7" t="n">
+        <v>1524414</v>
       </c>
       <c r="G13" s="3" t="n">
         <v>2.06498133986657</v>
@@ -8585,14 +8590,14 @@
         <v>4.0919407938658</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>2019</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="6" t="n">
+      <c r="C14" s="7" t="n">
         <v>18812</v>
       </c>
       <c r="D14" s="3" t="n">
@@ -8601,8 +8606,8 @@
       <c r="E14" s="3" t="n">
         <v>3.33954673681875</v>
       </c>
-      <c r="F14" s="6" t="n">
-        <v>1660177.94</v>
+      <c r="F14" s="7" t="n">
+        <v>1660178</v>
       </c>
       <c r="G14" s="3" t="n">
         <v>3.95844607597737</v>
@@ -8611,7 +8616,7 @@
         <v>4.73272709533155</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <f aca="false">A14</f>
         <v>2019</v>
@@ -8619,7 +8624,7 @@
       <c r="B15" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="6" t="n">
+      <c r="C15" s="7" t="n">
         <v>18365</v>
       </c>
       <c r="D15" s="3" t="n">
@@ -8628,8 +8633,8 @@
       <c r="E15" s="3" t="n">
         <v>4.11393168174466</v>
       </c>
-      <c r="F15" s="6" t="n">
-        <v>1599467.73</v>
+      <c r="F15" s="7" t="n">
+        <v>1599468</v>
       </c>
       <c r="G15" s="3" t="n">
         <v>3.35195870774942</v>
@@ -8638,7 +8643,7 @@
         <v>5.38237127042209</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <f aca="false">A15</f>
         <v>2019</v>
@@ -8646,7 +8651,7 @@
       <c r="B16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="6" t="n">
+      <c r="C16" s="7" t="n">
         <v>17101</v>
       </c>
       <c r="D16" s="3" t="n">
@@ -8655,8 +8660,8 @@
       <c r="E16" s="3" t="n">
         <v>4.90046988785815</v>
       </c>
-      <c r="F16" s="6" t="n">
-        <v>1522192.93</v>
+      <c r="F16" s="7" t="n">
+        <v>1522193</v>
       </c>
       <c r="G16" s="3" t="n">
         <v>3.57749778956074</v>
@@ -8665,7 +8670,7 @@
         <v>6.04021047540013</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <f aca="false">A16</f>
         <v>2019</v>
@@ -8673,7 +8678,7 @@
       <c r="B17" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C17" s="7" t="n">
         <v>15887</v>
       </c>
       <c r="D17" s="3" t="n">
@@ -8682,8 +8687,8 @@
       <c r="E17" s="3" t="n">
         <v>5.69786825552171</v>
       </c>
-      <c r="F17" s="6" t="n">
-        <v>1468852.65</v>
+      <c r="F17" s="7" t="n">
+        <v>1468853</v>
       </c>
       <c r="G17" s="3" t="n">
         <v>4.9558710251193</v>
@@ -8692,7 +8697,7 @@
         <v>6.70544086565598</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <f aca="false">A17</f>
         <v>2019</v>
@@ -8700,7 +8705,7 @@
       <c r="B18" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C18" s="6" t="n">
+      <c r="C18" s="7" t="n">
         <v>15918</v>
       </c>
       <c r="D18" s="3" t="n">
@@ -8709,8 +8714,8 @@
       <c r="E18" s="3" t="n">
         <v>6.50464440401188</v>
       </c>
-      <c r="F18" s="6" t="n">
-        <v>1457503.99</v>
+      <c r="F18" s="7" t="n">
+        <v>1457504</v>
       </c>
       <c r="G18" s="3" t="n">
         <v>8.46767821622381</v>
@@ -8719,7 +8724,7 @@
         <v>7.37708757486564</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <f aca="false">A18</f>
         <v>2019</v>
@@ -8727,7 +8732,7 @@
       <c r="B19" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C19" s="6" t="n">
+      <c r="C19" s="7" t="n">
         <v>14847</v>
       </c>
       <c r="D19" s="3" t="n">
@@ -8736,8 +8741,8 @@
       <c r="E19" s="3" t="n">
         <v>7.31907168013876</v>
       </c>
-      <c r="F19" s="6" t="n">
-        <v>1429088.15</v>
+      <c r="F19" s="7" t="n">
+        <v>1429088</v>
       </c>
       <c r="G19" s="3" t="n">
         <v>8.35574954697163</v>
@@ -8746,7 +8751,7 @@
         <v>8.05405423879953</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <f aca="false">A19</f>
         <v>2019</v>
@@ -8754,7 +8759,7 @@
       <c r="B20" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C20" s="6" t="n">
+      <c r="C20" s="7" t="n">
         <v>14556</v>
       </c>
       <c r="D20" s="3" t="n">
@@ -8763,8 +8768,8 @@
       <c r="E20" s="3" t="n">
         <v>8.13965820586491</v>
       </c>
-      <c r="F20" s="6" t="n">
-        <v>1567229.72</v>
+      <c r="F20" s="7" t="n">
+        <v>1567230</v>
       </c>
       <c r="G20" s="3" t="n">
         <v>11.8657902071124</v>
@@ -8773,7 +8778,7 @@
         <v>8.73532022868927</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <f aca="false">A20</f>
         <v>2019</v>
@@ -8781,7 +8786,7 @@
       <c r="B21" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C21" s="6" t="n">
+      <c r="C21" s="7" t="n">
         <v>15254</v>
       </c>
       <c r="D21" s="3" t="n">
@@ -8790,8 +8795,8 @@
       <c r="E21" s="3" t="n">
         <v>8.96497975210777</v>
       </c>
-      <c r="F21" s="6" t="n">
-        <v>1661109.79</v>
+      <c r="F21" s="7" t="n">
+        <v>1661110</v>
       </c>
       <c r="G21" s="3" t="n">
         <v>10.501794933453</v>
@@ -8800,7 +8805,7 @@
         <v>9.41988586682954</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <f aca="false">A21</f>
         <v>2019</v>
@@ -8808,7 +8813,7 @@
       <c r="B22" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C22" s="6" t="n">
+      <c r="C22" s="7" t="n">
         <v>15512</v>
       </c>
       <c r="D22" s="3" t="n">
@@ -8817,8 +8822,8 @@
       <c r="E22" s="3" t="n">
         <v>9.7937032134152</v>
       </c>
-      <c r="F22" s="6" t="n">
-        <v>1590970.03</v>
+      <c r="F22" s="7" t="n">
+        <v>1590970</v>
       </c>
       <c r="G22" s="3" t="n">
         <v>11.5802453322004</v>
@@ -8827,7 +8832,7 @@
         <v>10.1069688692635</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <f aca="false">A22</f>
         <v>2019</v>
@@ -8835,7 +8840,7 @@
       <c r="B23" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C23" s="6" t="n">
+      <c r="C23" s="7" t="n">
         <v>16811</v>
       </c>
       <c r="D23" s="3" t="n">
@@ -8844,8 +8849,8 @@
       <c r="E23" s="3" t="n">
         <v>10.6245003485896</v>
       </c>
-      <c r="F23" s="6" t="n">
-        <v>1639199.01</v>
+      <c r="F23" s="7" t="n">
+        <v>1639199</v>
       </c>
       <c r="G23" s="3" t="n">
         <v>14.5418202836078</v>
@@ -8854,7 +8859,7 @@
         <v>10.7958620846085</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <f aca="false">A23</f>
         <v>2019</v>
@@ -8862,7 +8867,7 @@
       <c r="B24" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C24" s="6" t="n">
+      <c r="C24" s="7" t="n">
         <v>18014</v>
       </c>
       <c r="D24" s="3" t="n">
@@ -8871,8 +8876,8 @@
       <c r="E24" s="3" t="n">
         <v>11.4564723516335</v>
       </c>
-      <c r="F24" s="6" t="n">
-        <v>1701239.28</v>
+      <c r="F24" s="7" t="n">
+        <v>1701239</v>
       </c>
       <c r="G24" s="3" t="n">
         <v>12.856274411563</v>
@@ -8881,7 +8886,7 @@
         <v>11.4859606723472</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <f aca="false">A24</f>
         <v>2019</v>
@@ -8889,7 +8894,7 @@
       <c r="B25" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="C25" s="6" t="n">
+      <c r="C25" s="7" t="n">
         <v>18580</v>
       </c>
       <c r="D25" s="3" t="n">
@@ -8898,8 +8903,8 @@
       <c r="E25" s="3" t="n">
         <v>12.2891267797951</v>
       </c>
-      <c r="F25" s="6" t="n">
-        <v>1725934.43</v>
+      <c r="F25" s="7" t="n">
+        <v>1725934</v>
       </c>
       <c r="G25" s="3" t="n">
         <v>13.2195468208262</v>
@@ -8908,14 +8913,14 @@
         <v>12.1769199279484</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C26" s="6" t="n">
+      <c r="C26" s="7" t="n">
         <v>21237</v>
       </c>
       <c r="D26" s="3" t="n">
@@ -8924,8 +8929,8 @@
       <c r="E26" s="3" t="n">
         <v>13.1222718582675</v>
       </c>
-      <c r="F26" s="6" t="n">
-        <v>1867077.27</v>
+      <c r="F26" s="7" t="n">
+        <v>1867077</v>
       </c>
       <c r="G26" s="3" t="n">
         <v>12.4624791725639</v>
@@ -8934,7 +8939,7 @@
         <v>12.8684903075572</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <f aca="false">A26</f>
         <v>2020</v>
@@ -8942,8 +8947,8 @@
       <c r="B27" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C27" s="6" t="n">
-        <v>20710.68</v>
+      <c r="C27" s="7" t="n">
+        <v>20711</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>12.7725564933297</v>
@@ -8951,8 +8956,8 @@
       <c r="E27" s="3" t="n">
         <v>13.9557821469761</v>
       </c>
-      <c r="F27" s="6" t="n">
-        <v>1810993.26</v>
+      <c r="F27" s="7" t="n">
+        <v>1810993</v>
       </c>
       <c r="G27" s="3" t="n">
         <v>13.2247450844163</v>
@@ -8961,7 +8966,7 @@
         <v>13.5604946719641</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <f aca="false">A27</f>
         <v>2020</v>
@@ -8969,7 +8974,7 @@
       <c r="B28" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C28" s="6" t="n">
+      <c r="C28" s="7" t="n">
         <v>20181</v>
       </c>
       <c r="D28" s="3" t="n">
@@ -8978,8 +8983,8 @@
       <c r="E28" s="3" t="n">
         <v>14.7895161250268</v>
       </c>
-      <c r="F28" s="6" t="n">
-        <v>1789266.14</v>
+      <c r="F28" s="7" t="n">
+        <v>1789266</v>
       </c>
       <c r="G28" s="3" t="n">
         <v>17.5452930266862</v>
@@ -8988,36 +8993,6 @@
         <v>14.2527276867419</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update monthly series: Tráfico de pasajeros
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_mensual.xlsx
+++ b/etl/data/input/Datos_carga_mensual.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" firstSheet="13" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Paro" sheetId="2" r:id="rId1"/>
@@ -4353,8 +4353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4407,19 +4407,19 @@
         <v>65228</v>
       </c>
       <c r="D2" s="3">
-        <v>36.377511551569143</v>
+        <v>36.380000000000003</v>
       </c>
       <c r="E2" s="3">
-        <v>15.157721847543051</v>
+        <v>15.51</v>
       </c>
       <c r="F2" s="4">
         <v>15439744</v>
       </c>
       <c r="G2" s="3">
-        <v>8.8193559577506075</v>
+        <v>8.82</v>
       </c>
       <c r="H2" s="3">
-        <v>8.069772662558881</v>
+        <v>8.41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -4433,19 +4433,19 @@
         <v>64052</v>
       </c>
       <c r="D3" s="3">
-        <v>32.412709569387886</v>
+        <v>32.409999999999997</v>
       </c>
       <c r="E3" s="3">
-        <v>15.213516860693929</v>
+        <v>15.45</v>
       </c>
       <c r="F3" s="4">
         <v>15229574</v>
       </c>
       <c r="G3" s="3">
-        <v>9.2852587212506332</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="H3" s="3">
-        <v>7.8233875215210054</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4459,19 +4459,19 @@
         <v>77644</v>
       </c>
       <c r="D4" s="3">
-        <v>23.334498205038589</v>
+        <v>23.33</v>
       </c>
       <c r="E4" s="3">
-        <v>15.194424723795084</v>
+        <v>15.29</v>
       </c>
       <c r="F4" s="4">
         <v>19042867</v>
       </c>
       <c r="G4" s="3">
-        <v>11.010748174996321</v>
+        <v>11.01</v>
       </c>
       <c r="H4" s="3">
-        <v>7.558449544956078</v>
+        <v>7.65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4485,19 +4485,19 @@
         <v>93701</v>
       </c>
       <c r="D5" s="3">
-        <v>11.53818683934864</v>
+        <v>11.54</v>
       </c>
       <c r="E5" s="3">
-        <v>15.102229538793829</v>
+        <v>15.05</v>
       </c>
       <c r="F5" s="4">
         <v>21595507</v>
       </c>
       <c r="G5" s="3">
-        <v>2.926911454907688</v>
+        <v>2.93</v>
       </c>
       <c r="H5" s="3">
-        <v>7.2749065653695499</v>
+        <v>7.22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4511,19 +4511,19 @@
         <v>98149</v>
       </c>
       <c r="D6" s="3">
-        <v>18.474482159239059</v>
+        <v>18.47</v>
       </c>
       <c r="E6" s="3">
-        <v>14.939280690518117</v>
+        <v>14.71</v>
       </c>
       <c r="F6" s="4">
         <v>23766470</v>
       </c>
       <c r="G6" s="3">
-        <v>6.4043820224115366</v>
+        <v>6.4</v>
       </c>
       <c r="H6" s="3">
-        <v>6.9729461582272929</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -4537,19 +4537,19 @@
         <v>101358</v>
       </c>
       <c r="D7" s="3">
-        <v>11.785336156696658</v>
+        <v>11.79</v>
       </c>
       <c r="E7" s="3">
-        <v>14.707680060830668</v>
+        <v>14.28</v>
       </c>
       <c r="F7" s="4">
         <v>25701475</v>
       </c>
       <c r="G7" s="3">
-        <v>5.094535287390678</v>
+        <v>5.09</v>
       </c>
       <c r="H7" s="3">
-        <v>6.6524539548902872</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4563,19 +4563,19 @@
         <v>118100</v>
       </c>
       <c r="D8" s="3">
-        <v>14.514549456516468</v>
+        <v>14.51</v>
       </c>
       <c r="E8" s="3">
-        <v>14.409775031696197</v>
+        <v>13.76</v>
       </c>
       <c r="F8" s="4">
         <v>28398012</v>
       </c>
       <c r="G8" s="3">
-        <v>3.1711472297570431</v>
+        <v>3.17</v>
       </c>
       <c r="H8" s="3">
-        <v>6.3132761030989695</v>
+        <v>5.68</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -4589,19 +4589,19 @@
         <v>114345</v>
       </c>
       <c r="D9" s="3">
-        <v>9.1286505058217227</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="E9" s="3">
-        <v>14.04771004453052</v>
+        <v>13.15</v>
       </c>
       <c r="F9" s="4">
         <v>28301898</v>
       </c>
       <c r="G9" s="3">
-        <v>3.346719304960688</v>
+        <v>3.35</v>
       </c>
       <c r="H9" s="3">
-        <v>5.9551505617974225</v>
+        <v>5.09</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -4615,19 +4615,19 @@
         <v>105440</v>
       </c>
       <c r="D10" s="3">
-        <v>22.058227701568555</v>
+        <v>22.06</v>
       </c>
       <c r="E10" s="3">
-        <v>13.623636816751175</v>
+        <v>12.45</v>
       </c>
       <c r="F10" s="4">
         <v>26202347</v>
       </c>
       <c r="G10" s="3">
-        <v>4.6420319055328507</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="H10" s="3">
-        <v>5.5775970865357465</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -4641,19 +4641,19 @@
         <v>101294</v>
       </c>
       <c r="D11" s="3">
-        <v>18.939927668968103</v>
+        <v>18.940000000000001</v>
       </c>
       <c r="E11" s="3">
-        <v>13.139365464418843</v>
+        <v>11.67</v>
       </c>
       <c r="F11" s="4">
         <v>24286809</v>
       </c>
       <c r="G11" s="3">
-        <v>6.5280724973820758</v>
+        <v>6.53</v>
       </c>
       <c r="H11" s="3">
-        <v>5.1799542918045409</v>
+        <v>3.76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -4667,19 +4667,19 @@
         <v>82363</v>
       </c>
       <c r="D12" s="3">
-        <v>15.210731720964056</v>
+        <v>15.21</v>
       </c>
       <c r="E12" s="3">
-        <v>12.597291839072323</v>
+        <v>10.79</v>
       </c>
       <c r="F12" s="4">
         <v>17682154</v>
       </c>
       <c r="G12" s="3">
-        <v>6.9851588275903431</v>
+        <v>6.99</v>
       </c>
       <c r="H12" s="3">
-        <v>4.7614958222901684</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -4693,19 +4693,19 @@
         <v>81679</v>
       </c>
       <c r="D13" s="3">
-        <v>16.660953523580989</v>
+        <v>16.66</v>
       </c>
       <c r="E13" s="3">
-        <v>12.000214609070172</v>
+        <v>9.84</v>
       </c>
       <c r="F13" s="4">
         <v>17561320</v>
       </c>
       <c r="G13" s="3">
-        <v>7.7088534499968775</v>
+        <v>7.71</v>
       </c>
       <c r="H13" s="3">
-        <v>4.3215889419988232</v>
+        <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -4719,19 +4719,19 @@
         <v>75022</v>
       </c>
       <c r="D14" s="3">
-        <v>15.015024222726447</v>
+        <v>15.02</v>
       </c>
       <c r="E14" s="3">
-        <v>11.35111393165163</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F14" s="4">
         <v>16545292</v>
       </c>
       <c r="G14" s="3">
-        <v>7.1604036958125672</v>
+        <v>7.16</v>
       </c>
       <c r="H14" s="3">
-        <v>3.8597553359787349</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -4745,19 +4745,19 @@
         <v>74131</v>
       </c>
       <c r="D15" s="3">
-        <v>15.735652282520451</v>
+        <v>15.74</v>
       </c>
       <c r="E15" s="3">
-        <v>10.653293626480556</v>
+        <v>7.68</v>
       </c>
       <c r="F15" s="4">
-        <v>16217533</v>
+        <v>16217594</v>
       </c>
       <c r="G15" s="3">
-        <v>6.487108569156308</v>
+        <v>6.49</v>
       </c>
       <c r="H15" s="3">
-        <v>3.3757519159800773</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -4771,19 +4771,19 @@
         <v>89789</v>
       </c>
       <c r="D16" s="3">
-        <v>15.641904075009005</v>
+        <v>15.64</v>
       </c>
       <c r="E16" s="3">
-        <v>9.9103119514354656</v>
+        <v>6.49</v>
       </c>
       <c r="F16" s="4">
         <v>19923942</v>
       </c>
       <c r="G16" s="3">
-        <v>4.6267980551457866</v>
+        <v>4.63</v>
       </c>
       <c r="H16" s="3">
-        <v>2.8695648054446785</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -4797,19 +4797,19 @@
         <v>96807</v>
       </c>
       <c r="D17" s="3">
-        <v>3.3147992017160899</v>
+        <v>3.31</v>
       </c>
       <c r="E17" s="3">
-        <v>9.1260801059682102</v>
+        <v>5.22</v>
       </c>
       <c r="F17" s="4">
         <v>23159946</v>
       </c>
       <c r="G17" s="3">
-        <v>7.2442800254701067</v>
+        <v>7.24</v>
       </c>
       <c r="H17" s="3">
-        <v>2.3413961942486154</v>
+        <v>-1.41</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -4823,19 +4823,19 @@
         <v>98895</v>
       </c>
       <c r="D18" s="3">
-        <v>0.76006887487392039</v>
+        <v>0.76</v>
       </c>
       <c r="E18" s="3">
-        <v>8.3049073167614438</v>
+        <v>3.89</v>
       </c>
       <c r="F18" s="4">
         <v>24586068</v>
       </c>
       <c r="G18" s="3">
-        <v>3.448547470448915</v>
+        <v>3.45</v>
       </c>
       <c r="H18" s="3">
-        <v>1.7915703023547505</v>
+        <v>-2.46</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -4849,19 +4849,19 @@
         <v>106680</v>
       </c>
       <c r="D19" s="3">
-        <v>5.2506955543716316</v>
+        <v>5.25</v>
       </c>
       <c r="E19" s="3">
-        <v>7.4506992493239119</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="F19" s="4">
         <v>27224266</v>
       </c>
       <c r="G19" s="3">
-        <v>5.9249167606139297</v>
+        <v>5.92</v>
       </c>
       <c r="H19" s="3">
-        <v>1.2207518277697804</v>
+        <v>-3.56</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -4875,19 +4875,19 @@
         <v>123005</v>
       </c>
       <c r="D20" s="3">
-        <v>4.1532599491955979</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="E20" s="3">
-        <v>6.5668376220503397</v>
+        <v>1.03</v>
       </c>
       <c r="F20" s="4">
         <v>29361913</v>
       </c>
       <c r="G20" s="3">
-        <v>3.3942552034980533</v>
+        <v>3.39</v>
       </c>
       <c r="H20" s="3">
-        <v>0.62972053635929792</v>
+        <v>-4.7</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -4901,19 +4901,19 @@
         <v>120979</v>
       </c>
       <c r="D21" s="3">
-        <v>5.8017403471948947</v>
+        <v>5.8</v>
       </c>
       <c r="E21" s="3">
-        <v>5.6565513753010794</v>
+        <v>-0.49</v>
       </c>
       <c r="F21" s="4">
         <v>29427057</v>
       </c>
       <c r="G21" s="3">
-        <v>3.9755602256781541</v>
+        <v>3.98</v>
       </c>
       <c r="H21" s="3">
-        <v>1.9582872109231722E-2</v>
+        <v>-5.9</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -4927,19 +4927,19 @@
         <v>107101</v>
       </c>
       <c r="D22" s="3">
-        <v>1.5753034901365703</v>
+        <v>1.58</v>
       </c>
       <c r="E22" s="3">
-        <v>4.7229018398758669</v>
+        <v>-2.06</v>
       </c>
       <c r="F22" s="4">
         <v>27089279</v>
       </c>
       <c r="G22" s="3">
-        <v>3.3849334183689628</v>
+        <v>3.38</v>
       </c>
       <c r="H22" s="3">
-        <v>-0.60836273942038244</v>
+        <v>-7.14</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -4953,19 +4953,19 @@
         <v>102260</v>
       </c>
       <c r="D23" s="3">
-        <v>0.95365964420399685</v>
+        <v>0.95</v>
       </c>
       <c r="E23" s="3">
-        <v>3.7689604291419325</v>
+        <v>-3.68</v>
       </c>
       <c r="F23" s="4">
         <v>24662007</v>
       </c>
       <c r="G23" s="3">
-        <v>1.5448633041911686</v>
+        <v>1.54</v>
       </c>
       <c r="H23" s="3">
-        <v>-1.2525431520199555</v>
+        <v>-8.42</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -4979,19 +4979,19 @@
         <v>88558</v>
       </c>
       <c r="D24" s="3">
-        <v>7.5215812925707004</v>
+        <v>7.52</v>
       </c>
       <c r="E24" s="3">
-        <v>2.7975799732477751</v>
+        <v>-5.34</v>
       </c>
       <c r="F24" s="4">
         <v>18317324</v>
       </c>
       <c r="G24" s="3">
-        <v>3.5921528564902161</v>
+        <v>3.59</v>
       </c>
       <c r="H24" s="3">
-        <v>-1.9111079072467185</v>
+        <v>-9.74</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -5005,19 +5005,19 @@
         <v>87669</v>
       </c>
       <c r="D25" s="3">
-        <v>7.3335863563461778</v>
+        <v>7.33</v>
       </c>
       <c r="E25" s="3">
-        <v>1.8114177953429391</v>
+        <v>-7.03</v>
       </c>
       <c r="F25" s="4">
         <v>18207055</v>
       </c>
       <c r="G25" s="3">
-        <v>3.6770299726899713</v>
+        <v>3.68</v>
       </c>
       <c r="H25" s="3">
-        <v>-2.5820122823206657</v>
+        <v>-11.1</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -5031,19 +5031,19 @@
         <v>83192</v>
       </c>
       <c r="D26" s="3">
-        <v>10.890138892591516</v>
+        <v>10.89</v>
       </c>
       <c r="E26" s="3">
-        <v>0.81345927422414455</v>
+        <v>-8.76</v>
       </c>
       <c r="F26" s="4">
         <v>16935024</v>
       </c>
       <c r="G26" s="3">
-        <v>2.3555462182232922</v>
+        <v>2.36</v>
       </c>
       <c r="H26" s="3">
-        <v>-3.2628293835754207</v>
+        <v>-12.48</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -5057,19 +5057,19 @@
         <v>77086</v>
       </c>
       <c r="D27" s="3">
-        <v>3.9861866155859182</v>
+        <v>3.99</v>
       </c>
       <c r="E27" s="3">
-        <v>-0.19292672738404171</v>
+        <v>-10.52</v>
       </c>
       <c r="F27" s="4">
         <v>16855997</v>
       </c>
       <c r="G27" s="3">
-        <v>3.9368749858563534</v>
+        <v>3.94</v>
       </c>
       <c r="H27" s="3">
-        <v>-3.9506976616324527</v>
+        <v>-13.89</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -5083,26 +5083,46 @@
         <v>32350</v>
       </c>
       <c r="D28" s="3">
-        <v>-63.971087772444292</v>
+        <v>-63.97</v>
       </c>
       <c r="E28" s="3">
-        <v>-1.2036715773391102</v>
+        <v>-12.28</v>
       </c>
       <c r="F28" s="4">
         <v>8098161</v>
       </c>
       <c r="G28" s="3">
-        <v>-59.354624702280304</v>
+        <v>-59.35</v>
       </c>
       <c r="H28" s="3">
-        <v>-4.6423654021408831</v>
+        <v>-15.31</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="A29" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2">
+        <v>18</v>
+      </c>
+      <c r="D29" s="3">
+        <v>-99.98</v>
+      </c>
+      <c r="E29" s="3">
+        <v>-14.06</v>
+      </c>
+      <c r="F29" s="4">
+        <v>127770</v>
+      </c>
+      <c r="G29" s="3">
+        <v>-99.45</v>
+      </c>
+      <c r="H29" s="3">
+        <v>-16.739999999999998</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D30" s="3"/>
@@ -16025,7 +16045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -17222,7 +17242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -18419,7 +18439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -19616,7 +19636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Monthly and quarterly updates
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_mensual.xlsx
+++ b/etl/data/input/Datos_carga_mensual.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" firstSheet="10" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Paro" sheetId="2" r:id="rId1"/>
@@ -10500,8 +10500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -10557,7 +10557,7 @@
         <v>15.7</v>
       </c>
       <c r="E2" s="3">
-        <v>5.3879250733383746</v>
+        <v>5.4741426564528464</v>
       </c>
       <c r="F2" s="6">
         <v>105.313</v>
@@ -10566,7 +10566,7 @@
         <v>3.3</v>
       </c>
       <c r="H2" s="3">
-        <v>2.0216888363948913</v>
+        <v>2.1231505208752339</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -10583,7 +10583,7 @@
         <v>13.1</v>
       </c>
       <c r="E3" s="3">
-        <v>5.2359064447348471</v>
+        <v>5.3012506642627697</v>
       </c>
       <c r="F3" s="6">
         <v>104.06</v>
@@ -10592,7 +10592,7 @@
         <v>2.8</v>
       </c>
       <c r="H3" s="3">
-        <v>1.8848159458502216</v>
+        <v>1.9632727763449573</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -10609,7 +10609,7 @@
         <v>1.2</v>
       </c>
       <c r="E4" s="3">
-        <v>5.0440063048093586</v>
+        <v>5.0850188223942805</v>
       </c>
       <c r="F4" s="6">
         <v>110.46599999999999</v>
@@ -10618,7 +10618,7 @@
         <v>-3.7</v>
       </c>
       <c r="H4" s="3">
-        <v>1.7359353006814102</v>
+        <v>1.7875185434214398</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -10635,7 +10635,7 @@
         <v>11.8</v>
       </c>
       <c r="E5" s="3">
-        <v>4.8124608013926817</v>
+        <v>4.8254228211888481</v>
       </c>
       <c r="F5" s="6">
         <v>105.31699999999999</v>
@@ -10644,7 +10644,7 @@
         <v>11.1</v>
       </c>
       <c r="H5" s="3">
-        <v>1.5749376816630527</v>
+        <v>1.5954841659484447</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -10661,7 +10661,7 @@
         <v>7.9</v>
       </c>
       <c r="E6" s="3">
-        <v>4.5412391374333101</v>
+        <v>4.5221685580141653</v>
       </c>
       <c r="F6" s="6">
         <v>112.755</v>
@@ -10670,7 +10670,7 @@
         <v>1.2</v>
       </c>
       <c r="H6" s="3">
-        <v>1.4013363740627525</v>
+        <v>1.3863849100931087</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -10687,7 +10687,7 @@
         <v>5.5</v>
       </c>
       <c r="E7" s="3">
-        <v>4.2307957616574203</v>
+        <v>4.1754462758753421</v>
       </c>
       <c r="F7" s="6">
         <v>108.622</v>
@@ -10696,7 +10696,7 @@
         <v>-2.2000000000000002</v>
       </c>
       <c r="H7" s="3">
-        <v>1.2153061258091085</v>
+        <v>1.1600960778443774</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -10713,7 +10713,7 @@
         <v>11.2</v>
       </c>
       <c r="E8" s="3">
-        <v>3.8818183700733098</v>
+        <v>3.7856807894054034</v>
       </c>
       <c r="F8" s="6">
         <v>110.83499999999999</v>
@@ -10722,7 +10722,7 @@
         <v>3.6</v>
       </c>
       <c r="H8" s="3">
-        <v>1.017007703138076</v>
+        <v>0.91648002779466176</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -10739,7 +10739,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E9" s="3">
-        <v>3.4950827978724948</v>
+        <v>3.3533888961348843</v>
       </c>
       <c r="F9" s="6">
         <v>86.762</v>
@@ -10748,7 +10748,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="3">
-        <v>0.80636469824909562</v>
+        <v>0.65516577853096691</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -10765,7 +10765,7 @@
         <v>3.6</v>
       </c>
       <c r="E10" s="3">
-        <v>3.0718730873041262</v>
+        <v>2.8796022768728329</v>
       </c>
       <c r="F10" s="6">
         <v>103.342</v>
@@ -10774,7 +10774,7 @@
         <v>-2.9</v>
       </c>
       <c r="H10" s="3">
-        <v>0.58348007780666766</v>
+        <v>0.37596870419392314</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -10791,7 +10791,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="E11" s="3">
-        <v>2.6135152887563922</v>
+        <v>2.3654044604216216</v>
       </c>
       <c r="F11" s="6">
         <v>113.554</v>
@@ -10800,7 +10800,7 @@
         <v>3.7</v>
       </c>
       <c r="H11" s="3">
-        <v>0.34847025537124759</v>
+        <v>7.8728125745096258E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -10817,7 +10817,7 @@
         <v>-2</v>
       </c>
       <c r="E12" s="3">
-        <v>2.1213721280975295</v>
+        <v>1.8119290032032853</v>
       </c>
       <c r="F12" s="6">
         <v>108.95699999999999</v>
@@ -10826,7 +10826,7 @@
         <v>-3.3</v>
       </c>
       <c r="H12" s="3">
-        <v>0.10120973616455436</v>
+        <v>-0.236944133680628</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -10843,7 +10843,7 @@
         <v>7.9</v>
       </c>
       <c r="E13" s="3">
-        <v>1.5971942815229452</v>
+        <v>1.2207146418856636</v>
       </c>
       <c r="F13" s="6">
         <v>92.974999999999994</v>
@@ -10852,7 +10852,7 @@
         <v>-4.2</v>
       </c>
       <c r="H13" s="3">
-        <v>-0.15819422947053824</v>
+        <v>-0.57118477373487397</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -10869,7 +10869,7 @@
         <v>-0.1</v>
       </c>
       <c r="E14" s="3">
-        <v>1.0424462188302617</v>
+        <v>0.5930353958447071</v>
       </c>
       <c r="F14" s="6">
         <v>107.589</v>
@@ -10878,7 +10878,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H14" s="3">
-        <v>-0.42987058631172342</v>
+        <v>-0.92434320628220479</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -10895,7 +10895,7 @@
         <v>-0.6</v>
       </c>
       <c r="E15" s="3">
-        <v>0.4590301046586624</v>
+        <v>-6.9370876282653676E-2</v>
       </c>
       <c r="F15" s="6">
         <v>104.14100000000001</v>
@@ -10904,7 +10904,7 @@
         <v>0.1</v>
       </c>
       <c r="H15" s="3">
-        <v>-0.71422896009298109</v>
+        <v>-1.297020844244563</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -10921,7 +10921,7 @@
         <v>-1.2</v>
       </c>
       <c r="E16" s="3">
-        <v>-0.1512312328956435</v>
+        <v>-0.7648144433175329</v>
       </c>
       <c r="F16" s="6">
         <v>110.276</v>
@@ -10930,7 +10930,7 @@
         <v>-0.2</v>
       </c>
       <c r="H16" s="3">
-        <v>-1.0114963466464639</v>
+        <v>-1.6896021322656769</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -10947,7 +10947,7 @@
         <v>-0.2</v>
       </c>
       <c r="E17" s="3">
-        <v>-0.78658850949371484</v>
+        <v>-1.4916424233257473</v>
       </c>
       <c r="F17" s="6">
         <v>103.20099999999999</v>
@@ -10956,7 +10956,7 @@
         <v>-2</v>
       </c>
       <c r="H17" s="3">
-        <v>-1.3218431981265404</v>
+        <v>-2.102374499652869</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -10973,7 +10973,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="3">
-        <v>-1.4453652719609928</v>
+        <v>-2.2482321555923277</v>
       </c>
       <c r="F18" s="6">
         <v>114.57</v>
@@ -10982,7 +10982,7 @@
         <v>1.6</v>
       </c>
       <c r="H18" s="3">
-        <v>-1.6453836127746173</v>
+        <v>-2.5355219311209436</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -10999,7 +10999,7 @@
         <v>-2.2000000000000002</v>
       </c>
       <c r="E19" s="3">
-        <v>-2.1258443318097595</v>
+        <v>-3.0328712820117967</v>
       </c>
       <c r="F19" s="6">
         <v>106.514</v>
@@ -11008,7 +11008,7 @@
         <v>-1.9</v>
       </c>
       <c r="H19" s="3">
-        <v>-1.9822787830544542</v>
+        <v>-2.9892213020444514</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -11025,7 +11025,7 @@
         <v>-0.9</v>
       </c>
       <c r="E20" s="3">
-        <v>-2.8261386835195221</v>
+        <v>-3.8436218728012057</v>
       </c>
       <c r="F20" s="6">
         <v>114.69799999999999</v>
@@ -11034,7 +11034,7 @@
         <v>3.5</v>
       </c>
       <c r="H20" s="3">
-        <v>-2.332464527567812</v>
+        <v>-3.4633622987749484</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -11051,7 +11051,7 @@
         <v>-8.8000000000000007</v>
       </c>
       <c r="E21" s="3">
-        <v>-3.544366471268968</v>
+        <v>-4.6784881598941324</v>
       </c>
       <c r="F21" s="6">
         <v>85.929000000000002</v>
@@ -11060,7 +11060,7 @@
         <v>-1</v>
       </c>
       <c r="H21" s="3">
-        <v>-2.6958709511120738</v>
+        <v>-3.9577589672957942</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -11077,7 +11077,7 @@
         <v>-2.7</v>
       </c>
       <c r="E22" s="3">
-        <v>-4.2785120796059832</v>
+        <v>-5.5352699570385431</v>
       </c>
       <c r="F22" s="6">
         <v>106.408</v>
@@ -11086,7 +11086,7 @@
         <v>3</v>
       </c>
       <c r="H22" s="3">
-        <v>-3.0720231262257638</v>
+        <v>-4.4717417867640448</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -11103,7 +11103,7 @@
         <v>-0.4</v>
       </c>
       <c r="E23" s="3">
-        <v>-5.0269248676290612</v>
+        <v>-6.412053294082412</v>
       </c>
       <c r="F23" s="6">
         <v>114.613</v>
@@ -11112,7 +11112,7 @@
         <v>0.9</v>
       </c>
       <c r="H23" s="3">
-        <v>-3.460328356631357</v>
+        <v>-5.0044358364084713</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -11129,7 +11129,7 @@
         <v>-0.3</v>
       </c>
       <c r="E24" s="3">
-        <v>-5.7878445755422794</v>
+        <v>-7.3067273071266978</v>
       </c>
       <c r="F24" s="6">
         <v>108.345</v>
@@ -11138,7 +11138,7 @@
         <v>-0.6</v>
       </c>
       <c r="H24" s="3">
-        <v>-3.8597722777786734</v>
+        <v>-5.5544473245004315</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -11155,7 +11155,7 @@
         <v>-12.7</v>
       </c>
       <c r="E25" s="3">
-        <v>-6.5591896293227947</v>
+        <v>-8.2167636285713801</v>
       </c>
       <c r="F25" s="6">
         <v>95.063000000000002</v>
@@ -11164,7 +11164,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H25" s="3">
-        <v>-4.2690377245372115</v>
+        <v>-6.1199724290448652</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -11181,7 +11181,7 @@
         <v>-5.3</v>
       </c>
       <c r="E26" s="3">
-        <v>-7.3384973546300181</v>
+        <v>-9.1391473125312199</v>
       </c>
       <c r="F26" s="6">
         <v>102.997</v>
@@ -11190,7 +11190,7 @@
         <v>-4.3</v>
       </c>
       <c r="H26" s="3">
-        <v>-4.6865811587016237</v>
+        <v>-6.6988632692047325</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -11207,7 +11207,7 @@
         <v>-9.4</v>
       </c>
       <c r="E27" s="3">
-        <v>-8.12373152228799</v>
+        <v>-10.071174748980104</v>
       </c>
       <c r="F27" s="6">
         <v>103.758</v>
@@ -11216,7 +11216,7 @@
         <v>-0.4</v>
       </c>
       <c r="H27" s="3">
-        <v>-5.1104098033356911</v>
+        <v>-7.2883941882798648</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -11227,22 +11227,22 @@
         <v>3</v>
       </c>
       <c r="C28" s="6">
-        <v>103.377</v>
+        <v>102.211</v>
       </c>
       <c r="D28" s="3">
-        <v>-15.1</v>
+        <v>-16.100000000000001</v>
       </c>
       <c r="E28" s="3">
-        <v>-8.912714340804456</v>
+        <v>-11.009875720439659</v>
       </c>
       <c r="F28" s="6">
-        <v>97.38</v>
+        <v>96.975999999999999</v>
       </c>
       <c r="G28" s="3">
-        <v>-11.7</v>
+        <v>-12.1</v>
       </c>
       <c r="H28" s="3">
-        <v>-5.5385040355893951</v>
+        <v>-7.8856729418430644</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -11253,31 +11253,49 @@
         <v>4</v>
       </c>
       <c r="C29" s="6">
-        <v>76.953000000000003</v>
+        <v>74.177000000000007</v>
       </c>
       <c r="D29" s="3">
-        <v>-33.6</v>
+        <v>-36</v>
       </c>
       <c r="E29" s="3">
-        <v>-9.7033566484425577</v>
+        <v>-11.952233400073945</v>
       </c>
       <c r="F29" s="6">
-        <v>68.498000000000005</v>
+        <v>67.994</v>
       </c>
       <c r="G29" s="3">
-        <v>-33.6</v>
+        <v>-34.1</v>
       </c>
       <c r="H29" s="3">
-        <v>-5.9685171208208203</v>
+        <v>-8.4873289247596144</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C30" s="6"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="A30" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="6">
+        <v>87.876999999999995</v>
+      </c>
+      <c r="D30" s="3">
+        <v>-27.2</v>
+      </c>
+      <c r="E30" s="3">
+        <v>-12.895584441899766</v>
+      </c>
+      <c r="F30" s="6">
+        <v>82.668000000000006</v>
+      </c>
+      <c r="G30" s="3">
+        <v>-27.8</v>
+      </c>
+      <c r="H30" s="3">
+        <v>-9.0902841934960605</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C31" s="6"/>
@@ -12732,7 +12750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add conditional rate and trend variables processing for quarterly data
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_mensual.xlsx
+++ b/etl/data/input/Datos_carga_mensual.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" firstSheet="10" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" firstSheet="18" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Paro" sheetId="2" r:id="rId1"/>
@@ -28,8 +28,8 @@
     <sheet name="EOAT" sheetId="21" r:id="rId14"/>
     <sheet name="IT" sheetId="22" r:id="rId15"/>
     <sheet name="PRD_B" sheetId="23" r:id="rId16"/>
-    <sheet name="PRD_G" sheetId="24" r:id="rId17"/>
-    <sheet name="IPI" sheetId="25" r:id="rId18"/>
+    <sheet name="IPI" sheetId="25" r:id="rId17"/>
+    <sheet name="PRD_G" sheetId="24" r:id="rId18"/>
     <sheet name="CP" sheetId="26" r:id="rId19"/>
     <sheet name="TPS_P" sheetId="27" r:id="rId20"/>
     <sheet name="TPS_M" sheetId="28" r:id="rId21"/>
@@ -370,24 +370,6 @@
     <t>Beneficiarios prestaciones por desempleos España. Tendencia</t>
   </si>
   <si>
-    <t>Gasto prestaciones por desempleo Cantabria</t>
-  </si>
-  <si>
-    <t>Gasto prestaciones por desempleo Cantabria. Var interanual</t>
-  </si>
-  <si>
-    <t>Gasto prestaciones por desempleo Cantabria. Tendencia</t>
-  </si>
-  <si>
-    <t>Gasto prestaciones por desempleos España</t>
-  </si>
-  <si>
-    <t>Gasto prestaciones por desempleos España. Var interanual</t>
-  </si>
-  <si>
-    <t>Gasto prestaciones por desempleos España. Tendencia</t>
-  </si>
-  <si>
     <t>Índice de Producción Industrial  Cantabria</t>
   </si>
   <si>
@@ -458,24 +440,6 @@
   </si>
   <si>
     <t>Tráfico portuario España. Tendencia</t>
-  </si>
-  <si>
-    <t>Sociedades mercantiles constituidas Cantabria</t>
-  </si>
-  <si>
-    <t>Sociedades mercantiles constituidas Cantabria. Var interanual</t>
-  </si>
-  <si>
-    <t>Sociedades mercantiles constituidas Cantabria. Tendencia</t>
-  </si>
-  <si>
-    <t>Sociedades mercantiles constituidas España</t>
-  </si>
-  <si>
-    <t>Sociedades mercantiles constituidas España. Var interanual</t>
-  </si>
-  <si>
-    <t>Sociedades mercantiles constituidas España. Tendencia</t>
   </si>
   <si>
     <t>Exportaciones Cantabria</t>
@@ -692,6 +656,42 @@
   </si>
   <si>
     <t>Deficit público CC.AA España. Tendencia</t>
+  </si>
+  <si>
+    <t>Gasto prestaciones por desempleo Cantabria</t>
+  </si>
+  <si>
+    <t>Gasto prestaciones por desempleo Cantabria. Var interanual</t>
+  </si>
+  <si>
+    <t>Gasto prestaciones por desempleo Cantabria. Tendencia</t>
+  </si>
+  <si>
+    <t>Gasto prestaciones por desempleos España</t>
+  </si>
+  <si>
+    <t>Gasto prestaciones por desempleos España. Var interanual</t>
+  </si>
+  <si>
+    <t>Gasto prestaciones por desempleos España. Tendencia</t>
+  </si>
+  <si>
+    <t>Sociedades mercantiles constituidas Cantabria</t>
+  </si>
+  <si>
+    <t>Sociedades mercantiles constituidas Cantabria. Var interanual</t>
+  </si>
+  <si>
+    <t>Sociedades mercantiles constituidas Cantabria. Tendencia</t>
+  </si>
+  <si>
+    <t>Sociedades mercantiles constituidas España</t>
+  </si>
+  <si>
+    <t>Sociedades mercantiles constituidas España. Var interanual</t>
+  </si>
+  <si>
+    <t>Sociedades mercantiles constituidas España. Tendencia</t>
   </si>
 </sst>
 </file>
@@ -8323,7 +8323,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -9465,8 +9465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:L51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -9516,22 +9516,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>18236</v>
+        <v>117.399</v>
       </c>
       <c r="D2" s="3">
-        <v>-4.8721961398017761</v>
+        <v>15.7</v>
       </c>
       <c r="E2" s="3">
-        <v>-5.6245761190892853</v>
+        <v>5.4741426564528464</v>
       </c>
       <c r="F2" s="6">
-        <v>1596963.02</v>
+        <v>105.313</v>
       </c>
       <c r="G2" s="3">
-        <v>-0.75486590211465421</v>
+        <v>3.3</v>
       </c>
       <c r="H2" s="3">
-        <v>-3.1315659672144482</v>
+        <v>2.1231505208752339</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -9542,22 +9542,22 @@
         <v>2</v>
       </c>
       <c r="C3" s="6">
-        <v>18656</v>
+        <v>116.422</v>
       </c>
       <c r="D3" s="3">
-        <v>-1.7277707543194243</v>
+        <v>13.1</v>
       </c>
       <c r="E3" s="3">
-        <v>-4.7515522533446015</v>
+        <v>5.3012506642627697</v>
       </c>
       <c r="F3" s="6">
-        <v>1547593.05</v>
+        <v>104.06</v>
       </c>
       <c r="G3" s="3">
-        <v>-1.1860555147865437</v>
+        <v>2.8</v>
       </c>
       <c r="H3" s="3">
-        <v>-2.3332918819848159</v>
+        <v>1.9632727763449573</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -9568,22 +9568,22 @@
         <v>3</v>
       </c>
       <c r="C4" s="6">
-        <v>16737</v>
+        <v>123.3</v>
       </c>
       <c r="D4" s="3">
-        <v>-4.3599999999999977</v>
+        <v>1.2</v>
       </c>
       <c r="E4" s="3">
-        <v>-3.8198609699627291</v>
+        <v>5.0850188223942805</v>
       </c>
       <c r="F4" s="6">
-        <v>1469617.4</v>
+        <v>110.46599999999999</v>
       </c>
       <c r="G4" s="3">
-        <v>-1.998959491473451</v>
+        <v>-3.7</v>
       </c>
       <c r="H4" s="3">
-        <v>-1.4839766709982776</v>
+        <v>1.7875185434214398</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -9594,22 +9594,22 @@
         <v>4</v>
       </c>
       <c r="C5" s="6">
-        <v>15548</v>
+        <v>116.188</v>
       </c>
       <c r="D5" s="3">
-        <v>-3.6440257808626697</v>
+        <v>11.8</v>
       </c>
       <c r="E5" s="3">
-        <v>-2.8257016917303974</v>
+        <v>4.8254228211888481</v>
       </c>
       <c r="F5" s="6">
-        <v>1399495.46</v>
+        <v>105.31699999999999</v>
       </c>
       <c r="G5" s="3">
-        <v>0.76723246049186233</v>
+        <v>11.1</v>
       </c>
       <c r="H5" s="3">
-        <v>-0.58043038651473744</v>
+        <v>1.5954841659484447</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -9620,22 +9620,22 @@
         <v>5</v>
       </c>
       <c r="C6" s="6">
-        <v>14486</v>
+        <v>119.526</v>
       </c>
       <c r="D6" s="3">
-        <v>-6.6563567240157218</v>
+        <v>7.9</v>
       </c>
       <c r="E6" s="3">
-        <v>-1.7653113510892005</v>
+        <v>4.5221685580141653</v>
       </c>
       <c r="F6" s="6">
-        <v>1343721.94</v>
+        <v>112.755</v>
       </c>
       <c r="G6" s="3">
-        <v>-0.88290300997564408</v>
+        <v>1.2</v>
       </c>
       <c r="H6" s="3">
-        <v>0.38050115651003424</v>
+        <v>1.3863849100931087</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -9646,22 +9646,22 @@
         <v>6</v>
       </c>
       <c r="C7" s="6">
-        <v>13710</v>
+        <v>117.364</v>
       </c>
       <c r="D7" s="3">
-        <v>-4.2798296446275197</v>
+        <v>5.5</v>
       </c>
       <c r="E7" s="3">
-        <v>-0.6349837085424771</v>
+        <v>4.1754462758753421</v>
       </c>
       <c r="F7" s="6">
-        <v>1318885.3899999999</v>
+        <v>108.622</v>
       </c>
       <c r="G7" s="3">
-        <v>-0.47470822576179961</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="H7" s="3">
-        <v>1.4020657308179758</v>
+        <v>1.1600960778443774</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -9672,22 +9672,22 @@
         <v>7</v>
       </c>
       <c r="C8" s="6">
-        <v>13299</v>
+        <v>113.51600000000001</v>
       </c>
       <c r="D8" s="3">
-        <v>-4.2548596112310992</v>
+        <v>11.2</v>
       </c>
       <c r="E8" s="3">
-        <v>0.56864781947775833</v>
+        <v>3.7856807894054034</v>
       </c>
       <c r="F8" s="6">
-        <v>1400991.06</v>
+        <v>110.83499999999999</v>
       </c>
       <c r="G8" s="3">
-        <v>-1.0143934468821114</v>
+        <v>3.6</v>
       </c>
       <c r="H8" s="3">
-        <v>2.487423372750575</v>
+        <v>0.91648002779466176</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -9698,22 +9698,22 @@
         <v>8</v>
       </c>
       <c r="C9" s="6">
-        <v>13990</v>
+        <v>103.02200000000001</v>
       </c>
       <c r="D9" s="3">
-        <v>-2.0788129068383898</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E9" s="3">
-        <v>1.8486967022383745</v>
+        <v>3.3533888961348843</v>
       </c>
       <c r="F9" s="6">
-        <v>1503242.36</v>
+        <v>86.762</v>
       </c>
       <c r="G9" s="3">
-        <v>-0.42131355212629007</v>
+        <v>1</v>
       </c>
       <c r="H9" s="3">
-        <v>3.6396037871245568</v>
+        <v>0.65516577853096691</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -9724,22 +9724,22 @@
         <v>9</v>
       </c>
       <c r="C10" s="6">
-        <v>13375</v>
+        <v>114.91200000000001</v>
       </c>
       <c r="D10" s="3">
-        <v>-4.1424783200745381</v>
+        <v>3.6</v>
       </c>
       <c r="E10" s="3">
-        <v>3.2079414432124409</v>
+        <v>2.8796022768728329</v>
       </c>
       <c r="F10" s="6">
-        <v>1425852.78</v>
+        <v>103.342</v>
       </c>
       <c r="G10" s="3">
-        <v>0.79841435216752021</v>
+        <v>-2.9</v>
       </c>
       <c r="H10" s="3">
-        <v>4.8613934970330597</v>
+        <v>0.37596870419392314</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -9750,22 +9750,22 @@
         <v>10</v>
       </c>
       <c r="C11" s="6">
-        <v>14433</v>
+        <v>122.11</v>
       </c>
       <c r="D11" s="3">
-        <v>-1.1979737130339507</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E11" s="3">
-        <v>4.6488878021501741</v>
+        <v>2.3654044604216216</v>
       </c>
       <c r="F11" s="6">
-        <v>1431092.16</v>
+        <v>113.554</v>
       </c>
       <c r="G11" s="3">
-        <v>0.80323949336891243</v>
+        <v>3.7</v>
       </c>
       <c r="H11" s="3">
-        <v>6.1552970174206632</v>
+        <v>7.8728125745096258E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -9776,22 +9776,22 @@
         <v>11</v>
       </c>
       <c r="C12" s="6">
-        <v>15558</v>
+        <v>113.795</v>
       </c>
       <c r="D12" s="3">
-        <v>1.8127085923696162</v>
+        <v>-2</v>
       </c>
       <c r="E12" s="3">
-        <v>6.173531092984895</v>
+        <v>1.8119290032032853</v>
       </c>
       <c r="F12" s="6">
-        <v>1507438.81</v>
+        <v>108.95699999999999</v>
       </c>
       <c r="G12" s="3">
-        <v>2.0512359295589588</v>
+        <v>-3.3</v>
       </c>
       <c r="H12" s="3">
-        <v>7.5235367119024419</v>
+        <v>-0.236944133680628</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -9802,22 +9802,22 @@
         <v>12</v>
       </c>
       <c r="C13" s="6">
-        <v>16407</v>
+        <v>106.81399999999999</v>
       </c>
       <c r="D13" s="3">
-        <v>0.97236753030955914</v>
+        <v>7.9</v>
       </c>
       <c r="E13" s="3">
-        <v>7.7834605976002598</v>
+        <v>1.2207146418856636</v>
       </c>
       <c r="F13" s="6">
-        <v>1524413.83</v>
+        <v>92.974999999999994</v>
       </c>
       <c r="G13" s="3">
-        <v>2.0649813398665673</v>
+        <v>-4.2</v>
       </c>
       <c r="H13" s="3">
-        <v>8.967963273432078</v>
+        <v>-0.57118477373487397</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -9828,22 +9828,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="6">
-        <v>18812</v>
+        <v>117.23699999999999</v>
       </c>
       <c r="D14" s="3">
-        <v>3.158587409519642</v>
+        <v>-0.1</v>
       </c>
       <c r="E14" s="3">
-        <v>9.4799627629840497</v>
+        <v>0.5930353958447071</v>
       </c>
       <c r="F14" s="6">
-        <v>1660177.94</v>
+        <v>107.589</v>
       </c>
       <c r="G14" s="3">
-        <v>3.9584460759773732</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H14" s="3">
-        <v>10.490047374075592</v>
+        <v>-0.92434320628220479</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -9854,22 +9854,22 @@
         <v>2</v>
       </c>
       <c r="C15" s="6">
-        <v>18365</v>
+        <v>115.667</v>
       </c>
       <c r="D15" s="3">
-        <v>-1.5598198970840471</v>
+        <v>-0.6</v>
       </c>
       <c r="E15" s="3">
-        <v>11.263851043549929</v>
+        <v>-6.9370876282653676E-2</v>
       </c>
       <c r="F15" s="6">
-        <v>1599467.73</v>
+        <v>104.14100000000001</v>
       </c>
       <c r="G15" s="3">
-        <v>3.3519587077494251</v>
+        <v>0.1</v>
       </c>
       <c r="H15" s="3">
-        <v>12.090780312153621</v>
+        <v>-1.297020844244563</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -9880,22 +9880,22 @@
         <v>3</v>
       </c>
       <c r="C16" s="6">
-        <v>17101</v>
+        <v>121.816</v>
       </c>
       <c r="D16" s="3">
-        <v>2.1748222501045689</v>
+        <v>-1.2</v>
       </c>
       <c r="E16" s="3">
-        <v>13.135499909312017</v>
+        <v>-0.7648144433175329</v>
       </c>
       <c r="F16" s="6">
-        <v>1522192.93</v>
+        <v>110.276</v>
       </c>
       <c r="G16" s="3">
-        <v>3.5774977895607352</v>
+        <v>-0.2</v>
       </c>
       <c r="H16" s="3">
-        <v>13.770699802563316</v>
+        <v>-1.6896021322656769</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -9906,22 +9906,22 @@
         <v>4</v>
       </c>
       <c r="C17" s="6">
-        <v>15887</v>
+        <v>115.917</v>
       </c>
       <c r="D17" s="3">
-        <v>2.1803447388731634</v>
+        <v>-0.2</v>
       </c>
       <c r="E17" s="3">
-        <v>15.094393297580222</v>
+        <v>-1.4916424233257473</v>
       </c>
       <c r="F17" s="6">
-        <v>1468852.65</v>
+        <v>103.20099999999999</v>
       </c>
       <c r="G17" s="3">
-        <v>4.9558710251192961</v>
+        <v>-2</v>
       </c>
       <c r="H17" s="3">
-        <v>15.529736697590412</v>
+        <v>-2.102374499652869</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -9932,22 +9932,22 @@
         <v>5</v>
       </c>
       <c r="C18" s="6">
-        <v>15918</v>
+        <v>120.76</v>
       </c>
       <c r="D18" s="3">
-        <v>9.8854065994753668</v>
+        <v>1</v>
       </c>
       <c r="E18" s="3">
-        <v>17.139253987493674</v>
+        <v>-2.2482321555923277</v>
       </c>
       <c r="F18" s="6">
-        <v>1457503.99</v>
+        <v>114.57</v>
       </c>
       <c r="G18" s="3">
-        <v>8.4676782162238062</v>
+        <v>1.6</v>
       </c>
       <c r="H18" s="3">
-        <v>17.367113988269743</v>
+        <v>-2.5355219311209436</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -9958,22 +9958,22 @@
         <v>6</v>
       </c>
       <c r="C19" s="6">
-        <v>14847</v>
+        <v>114.836</v>
       </c>
       <c r="D19" s="3">
-        <v>8.2932166301969303</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="E19" s="3">
-        <v>19.267907949263819</v>
+        <v>-3.0328712820117967</v>
       </c>
       <c r="F19" s="6">
-        <v>1429088.15</v>
+        <v>106.514</v>
       </c>
       <c r="G19" s="3">
-        <v>8.3557495469716248</v>
+        <v>-1.9</v>
       </c>
       <c r="H19" s="3">
-        <v>19.281320369408888</v>
+        <v>-2.9892213020444514</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -9984,22 +9984,22 @@
         <v>7</v>
       </c>
       <c r="C20" s="6">
-        <v>14556</v>
+        <v>112.47199999999999</v>
       </c>
       <c r="D20" s="3">
-        <v>9.451838484096541</v>
+        <v>-0.9</v>
       </c>
       <c r="E20" s="3">
-        <v>21.477677413700157</v>
+        <v>-3.8436218728012057</v>
       </c>
       <c r="F20" s="6">
-        <v>1567229.72</v>
+        <v>114.69799999999999</v>
       </c>
       <c r="G20" s="3">
-        <v>11.865790207112381</v>
+        <v>3.5</v>
       </c>
       <c r="H20" s="3">
-        <v>21.270226519442367</v>
+        <v>-3.4633622987749484</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -10010,22 +10010,22 @@
         <v>8</v>
       </c>
       <c r="C21" s="6">
-        <v>15254</v>
+        <v>93.984999999999999</v>
       </c>
       <c r="D21" s="3">
-        <v>9.0350250178699021</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="E21" s="3">
-        <v>23.765122480270591</v>
+        <v>-4.6784881598941324</v>
       </c>
       <c r="F21" s="6">
-        <v>1661109.79</v>
+        <v>85.929000000000002</v>
       </c>
       <c r="G21" s="3">
-        <v>10.501794933453045</v>
+        <v>-1</v>
       </c>
       <c r="H21" s="3">
-        <v>23.3309443966087</v>
+        <v>-3.9577589672957942</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -10036,22 +10036,22 @@
         <v>9</v>
       </c>
       <c r="C22" s="6">
-        <v>15512</v>
+        <v>111.84399999999999</v>
       </c>
       <c r="D22" s="3">
-        <v>15.977570093457949</v>
+        <v>-2.7</v>
       </c>
       <c r="E22" s="3">
-        <v>26.125968120739575</v>
+        <v>-5.5352699570385431</v>
       </c>
       <c r="F22" s="6">
-        <v>1590970.0299999998</v>
+        <v>106.408</v>
       </c>
       <c r="G22" s="3">
-        <v>11.580245332200413</v>
+        <v>3</v>
       </c>
       <c r="H22" s="3">
-        <v>25.459932873291379</v>
+        <v>-4.4717417867640448</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -10062,22 +10062,22 @@
         <v>10</v>
       </c>
       <c r="C23" s="6">
-        <v>16811</v>
+        <v>121.601</v>
       </c>
       <c r="D23" s="3">
-        <v>16.476131088477786</v>
+        <v>-0.4</v>
       </c>
       <c r="E23" s="3">
-        <v>28.554916383436677</v>
+        <v>-6.412053294082412</v>
       </c>
       <c r="F23" s="6">
-        <v>1639199.0100000002</v>
+        <v>114.613</v>
       </c>
       <c r="G23" s="3">
-        <v>14.541820283607754</v>
+        <v>0.9</v>
       </c>
       <c r="H23" s="3">
-        <v>27.652759908716732</v>
+        <v>-5.0044358364084713</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -10088,22 +10088,22 @@
         <v>11</v>
       </c>
       <c r="C24" s="6">
-        <v>18014</v>
+        <v>113.40900000000001</v>
       </c>
       <c r="D24" s="3">
-        <v>15.786090757166725</v>
+        <v>-0.3</v>
       </c>
       <c r="E24" s="3">
-        <v>31.045964566828463</v>
+        <v>-7.3067273071266978</v>
       </c>
       <c r="F24" s="6">
-        <v>1701239.28</v>
+        <v>108.345</v>
       </c>
       <c r="G24" s="3">
-        <v>12.856274411563007</v>
+        <v>-0.6</v>
       </c>
       <c r="H24" s="3">
-        <v>29.90402959492074</v>
+        <v>-5.5544473245004315</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -10114,22 +10114,22 @@
         <v>12</v>
       </c>
       <c r="C25" s="6">
-        <v>18580</v>
+        <v>93.247</v>
       </c>
       <c r="D25" s="3">
-        <v>13.244346925092954</v>
+        <v>-12.7</v>
       </c>
       <c r="E25" s="3">
-        <v>33.592271164847126</v>
+        <v>-8.2167636285713801</v>
       </c>
       <c r="F25" s="6">
-        <v>1725934.4300000002</v>
+        <v>95.063000000000002</v>
       </c>
       <c r="G25" s="3">
-        <v>13.219546820826199</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H25" s="3">
-        <v>32.207435542020967</v>
+        <v>-6.1199724290448652</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -10140,22 +10140,22 @@
         <v>1</v>
       </c>
       <c r="C26" s="6">
-        <v>21237</v>
+        <v>111.078</v>
       </c>
       <c r="D26" s="3">
-        <v>12.890708058685952</v>
+        <v>-5.3</v>
       </c>
       <c r="E26" s="3">
-        <v>36.185934957965856</v>
+        <v>-9.1391473125312199</v>
       </c>
       <c r="F26" s="6">
-        <v>1867077.27</v>
+        <v>102.997</v>
       </c>
       <c r="G26" s="3">
-        <v>12.462479172563889</v>
+        <v>-4.3</v>
       </c>
       <c r="H26" s="3">
-        <v>34.555487488247252</v>
+        <v>-6.6988632692047325</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -10166,22 +10166,22 @@
         <v>2</v>
       </c>
       <c r="C27" s="6">
-        <v>20710.68</v>
+        <v>104.83199999999999</v>
       </c>
       <c r="D27" s="3">
-        <v>12.772556493329713</v>
+        <v>-9.4</v>
       </c>
       <c r="E27" s="3">
-        <v>38.817641676363415</v>
+        <v>-10.071174748980104</v>
       </c>
       <c r="F27" s="6">
-        <v>1810993.2600000002</v>
+        <v>103.758</v>
       </c>
       <c r="G27" s="3">
-        <v>13.224745084416313</v>
+        <v>-0.4</v>
       </c>
       <c r="H27" s="3">
-        <v>36.939376568446015</v>
+        <v>-7.2883941882798648</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -10192,22 +10192,22 @@
         <v>3</v>
       </c>
       <c r="C28" s="6">
-        <v>20181</v>
+        <v>102.211</v>
       </c>
       <c r="D28" s="3">
-        <v>18.01064265247647</v>
+        <v>-16.100000000000001</v>
       </c>
       <c r="E28" s="3">
-        <v>41.476459326128335</v>
+        <v>-11.009875720439659</v>
       </c>
       <c r="F28" s="6">
-        <v>1789266.14</v>
+        <v>96.975999999999999</v>
       </c>
       <c r="G28" s="3">
-        <v>17.545293026686171</v>
+        <v>-12.1</v>
       </c>
       <c r="H28" s="3">
-        <v>39.348759680775089</v>
+        <v>-7.8856729418430644</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -10218,31 +10218,49 @@
         <v>4</v>
       </c>
       <c r="C29" s="6">
-        <v>55776.28</v>
+        <v>74.177000000000007</v>
       </c>
       <c r="D29" s="3">
-        <v>251.08126140869894</v>
+        <v>-36</v>
       </c>
       <c r="E29" s="3">
-        <v>44.149647226878102</v>
+        <v>-11.952233400073945</v>
       </c>
       <c r="F29" s="6">
-        <v>4938729.3099999996</v>
+        <v>67.994</v>
       </c>
       <c r="G29" s="3">
-        <v>236.23041153923779</v>
+        <v>-34.1</v>
       </c>
       <c r="H29" s="3">
-        <v>41.771646873983691</v>
+        <v>-8.4873289247596144</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C30" s="6"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="A30" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="6">
+        <v>87.876999999999995</v>
+      </c>
+      <c r="D30" s="3">
+        <v>-27.2</v>
+      </c>
+      <c r="E30" s="3">
+        <v>-12.895584441899766</v>
+      </c>
+      <c r="F30" s="6">
+        <v>82.668000000000006</v>
+      </c>
+      <c r="G30" s="3">
+        <v>-27.8</v>
+      </c>
+      <c r="H30" s="3">
+        <v>-9.0902841934960605</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C31" s="6"/>
@@ -10500,8 +10518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:H30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -10525,22 +10543,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>199</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>111</v>
+        <v>201</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>112</v>
+        <v>202</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>113</v>
+        <v>203</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>114</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -10551,22 +10569,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>117.399</v>
+        <v>18236</v>
       </c>
       <c r="D2" s="3">
-        <v>15.7</v>
+        <v>-4.8721961398017761</v>
       </c>
       <c r="E2" s="3">
-        <v>5.4741426564528464</v>
+        <v>-6.7709498404522019</v>
       </c>
       <c r="F2" s="6">
-        <v>105.313</v>
+        <v>1596963.02</v>
       </c>
       <c r="G2" s="3">
-        <v>3.3</v>
+        <v>-0.75486590211465421</v>
       </c>
       <c r="H2" s="3">
-        <v>2.1231505208752339</v>
+        <v>-4.2718529593201522</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -10577,22 +10595,22 @@
         <v>2</v>
       </c>
       <c r="C3" s="6">
-        <v>116.422</v>
+        <v>18656</v>
       </c>
       <c r="D3" s="3">
-        <v>13.1</v>
+        <v>-1.7277707543194243</v>
       </c>
       <c r="E3" s="3">
-        <v>5.3012506642627697</v>
+        <v>-5.6439089601113235</v>
       </c>
       <c r="F3" s="6">
-        <v>104.06</v>
+        <v>1547593.05</v>
       </c>
       <c r="G3" s="3">
-        <v>2.8</v>
+        <v>-1.1860555147865437</v>
       </c>
       <c r="H3" s="3">
-        <v>1.9632727763449573</v>
+        <v>-3.2286845907488715</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -10603,22 +10621,22 @@
         <v>3</v>
       </c>
       <c r="C4" s="6">
-        <v>123.3</v>
+        <v>16737</v>
       </c>
       <c r="D4" s="3">
-        <v>1.2</v>
+        <v>-4.3599999999999977</v>
       </c>
       <c r="E4" s="3">
-        <v>5.0850188223942805</v>
+        <v>-4.4152510197978803</v>
       </c>
       <c r="F4" s="6">
-        <v>110.46599999999999</v>
+        <v>1469617.4</v>
       </c>
       <c r="G4" s="3">
-        <v>-3.7</v>
+        <v>-1.998959491473451</v>
       </c>
       <c r="H4" s="3">
-        <v>1.7875185434214398</v>
+        <v>-2.0935955927178336</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -10629,22 +10647,22 @@
         <v>4</v>
       </c>
       <c r="C5" s="6">
-        <v>116.188</v>
+        <v>15548</v>
       </c>
       <c r="D5" s="3">
-        <v>11.8</v>
+        <v>-3.6440257808626697</v>
       </c>
       <c r="E5" s="3">
-        <v>4.8254228211888481</v>
+        <v>-3.0778944449047088</v>
       </c>
       <c r="F5" s="6">
-        <v>105.31699999999999</v>
+        <v>1399495.46</v>
       </c>
       <c r="G5" s="3">
-        <v>11.1</v>
+        <v>0.76723246049186233</v>
       </c>
       <c r="H5" s="3">
-        <v>1.5954841659484447</v>
+        <v>-0.86029109980880114</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -10655,22 +10673,22 @@
         <v>5</v>
       </c>
       <c r="C6" s="6">
-        <v>119.526</v>
+        <v>14486</v>
       </c>
       <c r="D6" s="3">
-        <v>7.9</v>
+        <v>-6.6563567240157218</v>
       </c>
       <c r="E6" s="3">
-        <v>4.5221685580141653</v>
+        <v>-1.6247538239482708</v>
       </c>
       <c r="F6" s="6">
-        <v>112.755</v>
+        <v>1343721.94</v>
       </c>
       <c r="G6" s="3">
-        <v>1.2</v>
+        <v>-0.88290300997564408</v>
       </c>
       <c r="H6" s="3">
-        <v>1.3863849100931087</v>
+        <v>0.47753032534793877</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -10681,22 +10699,22 @@
         <v>6</v>
       </c>
       <c r="C7" s="6">
-        <v>117.364</v>
+        <v>13710</v>
       </c>
       <c r="D7" s="3">
-        <v>5.5</v>
+        <v>-4.2798296446275197</v>
       </c>
       <c r="E7" s="3">
-        <v>4.1754462758753421</v>
+        <v>-4.8783060121136979E-2</v>
       </c>
       <c r="F7" s="6">
-        <v>108.622</v>
+        <v>1318885.3899999999</v>
       </c>
       <c r="G7" s="3">
-        <v>-2.2000000000000002</v>
+        <v>-0.47470822576179961</v>
       </c>
       <c r="H7" s="3">
-        <v>1.1600960778443774</v>
+        <v>1.9262831425915643</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -10707,22 +10725,22 @@
         <v>7</v>
       </c>
       <c r="C8" s="6">
-        <v>113.51600000000001</v>
+        <v>13299</v>
       </c>
       <c r="D8" s="3">
-        <v>11.2</v>
+        <v>-4.2548596112310992</v>
       </c>
       <c r="E8" s="3">
-        <v>3.7856807894054034</v>
+        <v>1.6567145265160628</v>
       </c>
       <c r="F8" s="6">
-        <v>110.83499999999999</v>
+        <v>1400991.06</v>
       </c>
       <c r="G8" s="3">
-        <v>3.6</v>
+        <v>-1.0143934468821114</v>
       </c>
       <c r="H8" s="3">
-        <v>0.91648002779466176</v>
+        <v>3.4922873372240781</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -10733,22 +10751,22 @@
         <v>8</v>
       </c>
       <c r="C9" s="6">
-        <v>103.02200000000001</v>
+        <v>13990</v>
       </c>
       <c r="D9" s="3">
-        <v>4.0999999999999996</v>
+        <v>-2.0788129068383898</v>
       </c>
       <c r="E9" s="3">
-        <v>3.3533888961348843</v>
+        <v>3.4981417932232186</v>
       </c>
       <c r="F9" s="6">
-        <v>86.762</v>
+        <v>1503242.36</v>
       </c>
       <c r="G9" s="3">
-        <v>1</v>
+        <v>-0.42131355212629007</v>
       </c>
       <c r="H9" s="3">
-        <v>0.65516577853096691</v>
+        <v>5.1816961590357913</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -10759,22 +10777,22 @@
         <v>9</v>
       </c>
       <c r="C10" s="6">
-        <v>114.91200000000001</v>
+        <v>13375</v>
       </c>
       <c r="D10" s="3">
-        <v>3.6</v>
+        <v>-4.1424783200745381</v>
       </c>
       <c r="E10" s="3">
-        <v>2.8796022768728329</v>
+        <v>5.481491071278433</v>
       </c>
       <c r="F10" s="6">
-        <v>103.342</v>
+        <v>1425852.78</v>
       </c>
       <c r="G10" s="3">
-        <v>-2.9</v>
+        <v>0.79841435216752021</v>
       </c>
       <c r="H10" s="3">
-        <v>0.37596870419392314</v>
+        <v>7.0003498938736728</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -10785,22 +10803,22 @@
         <v>10</v>
       </c>
       <c r="C11" s="6">
-        <v>122.11</v>
+        <v>14433</v>
       </c>
       <c r="D11" s="3">
-        <v>8.1999999999999993</v>
+        <v>-1.1979737130339507</v>
       </c>
       <c r="E11" s="3">
-        <v>2.3654044604216216</v>
+        <v>7.6123674034389701</v>
       </c>
       <c r="F11" s="6">
-        <v>113.554</v>
+        <v>1431092.16</v>
       </c>
       <c r="G11" s="3">
-        <v>3.7</v>
+        <v>0.80323949336891243</v>
       </c>
       <c r="H11" s="3">
-        <v>7.8728125745096258E-2</v>
+        <v>8.9536997296880827</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -10811,22 +10829,22 @@
         <v>11</v>
       </c>
       <c r="C12" s="6">
-        <v>113.795</v>
+        <v>15558</v>
       </c>
       <c r="D12" s="3">
-        <v>-2</v>
+        <v>1.8127085923696162</v>
       </c>
       <c r="E12" s="3">
-        <v>1.8119290032032853</v>
+        <v>9.8957075012543605</v>
       </c>
       <c r="F12" s="6">
-        <v>108.95699999999999</v>
+        <v>1507438.81</v>
       </c>
       <c r="G12" s="3">
-        <v>-3.3</v>
+        <v>2.0512359295589588</v>
       </c>
       <c r="H12" s="3">
-        <v>-0.236944133680628</v>
+        <v>11.046766164461207</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -10837,22 +10855,22 @@
         <v>12</v>
       </c>
       <c r="C13" s="6">
-        <v>106.81399999999999</v>
+        <v>16407</v>
       </c>
       <c r="D13" s="3">
-        <v>7.9</v>
+        <v>0.97236753030955914</v>
       </c>
       <c r="E13" s="3">
-        <v>1.2207146418856636</v>
+        <v>12.335836247029937</v>
       </c>
       <c r="F13" s="6">
-        <v>92.974999999999994</v>
+        <v>1524413.83</v>
       </c>
       <c r="G13" s="3">
-        <v>-4.2</v>
+        <v>2.0649813398665673</v>
       </c>
       <c r="H13" s="3">
-        <v>-0.57118477373487397</v>
+        <v>13.284003691992154</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -10863,22 +10881,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="6">
-        <v>117.23699999999999</v>
+        <v>18812</v>
       </c>
       <c r="D14" s="3">
-        <v>-0.1</v>
+        <v>3.158587409519642</v>
       </c>
       <c r="E14" s="3">
-        <v>0.5930353958447071</v>
+        <v>14.936517203702358</v>
       </c>
       <c r="F14" s="6">
-        <v>107.589</v>
+        <v>1660177.94</v>
       </c>
       <c r="G14" s="3">
-        <v>2.2000000000000002</v>
+        <v>3.9584460759773732</v>
       </c>
       <c r="H14" s="3">
-        <v>-0.92434320628220479</v>
+        <v>15.66924211648039</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -10889,22 +10907,22 @@
         <v>2</v>
       </c>
       <c r="C15" s="6">
-        <v>115.667</v>
+        <v>18365</v>
       </c>
       <c r="D15" s="3">
-        <v>-0.6</v>
+        <v>-1.5598198970840471</v>
       </c>
       <c r="E15" s="3">
-        <v>-6.9370876282653676E-2</v>
+        <v>17.700724804436295</v>
       </c>
       <c r="F15" s="6">
-        <v>104.14100000000001</v>
+        <v>1599467.73</v>
       </c>
       <c r="G15" s="3">
-        <v>0.1</v>
+        <v>3.3519587077494251</v>
       </c>
       <c r="H15" s="3">
-        <v>-1.297020844244563</v>
+        <v>18.205532143350926</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -10915,22 +10933,22 @@
         <v>3</v>
       </c>
       <c r="C16" s="6">
-        <v>121.816</v>
+        <v>17101</v>
       </c>
       <c r="D16" s="3">
-        <v>-1.2</v>
+        <v>2.1748222501045689</v>
       </c>
       <c r="E16" s="3">
-        <v>-0.7648144433175329</v>
+        <v>20.630615570605151</v>
       </c>
       <c r="F16" s="6">
-        <v>110.276</v>
+        <v>1522192.93</v>
       </c>
       <c r="G16" s="3">
-        <v>-0.2</v>
+        <v>3.5774977895607352</v>
       </c>
       <c r="H16" s="3">
-        <v>-1.6896021322656769</v>
+        <v>20.895111228303733</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -10941,22 +10959,22 @@
         <v>4</v>
       </c>
       <c r="C17" s="6">
-        <v>115.917</v>
+        <v>15887</v>
       </c>
       <c r="D17" s="3">
-        <v>-0.2</v>
+        <v>2.1803447388731634</v>
       </c>
       <c r="E17" s="3">
-        <v>-1.4916424233257473</v>
+        <v>23.727008485755839</v>
       </c>
       <c r="F17" s="6">
-        <v>103.20099999999999</v>
+        <v>1468852.65</v>
       </c>
       <c r="G17" s="3">
-        <v>-2</v>
+        <v>4.9558710251192961</v>
       </c>
       <c r="H17" s="3">
-        <v>-2.102374499652869</v>
+        <v>23.739185328883536</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -10967,22 +10985,22 @@
         <v>5</v>
       </c>
       <c r="C18" s="6">
-        <v>120.76</v>
+        <v>15918</v>
       </c>
       <c r="D18" s="3">
-        <v>1</v>
+        <v>9.8854065994753668</v>
       </c>
       <c r="E18" s="3">
-        <v>-2.2482321555923277</v>
+        <v>26.989440881121347</v>
       </c>
       <c r="F18" s="6">
-        <v>114.57</v>
+        <v>1457503.99</v>
       </c>
       <c r="G18" s="3">
-        <v>1.6</v>
+        <v>8.4676782162238062</v>
       </c>
       <c r="H18" s="3">
-        <v>-2.5355219311209436</v>
+        <v>26.737757790590702</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -10993,22 +11011,22 @@
         <v>6</v>
       </c>
       <c r="C19" s="6">
-        <v>114.836</v>
+        <v>14847</v>
       </c>
       <c r="D19" s="3">
-        <v>-2.2000000000000002</v>
+        <v>8.2932166301969303</v>
       </c>
       <c r="E19" s="3">
-        <v>-3.0328712820117967</v>
+        <v>30.415953791841133</v>
       </c>
       <c r="F19" s="6">
-        <v>106.514</v>
+        <v>1429088.15</v>
       </c>
       <c r="G19" s="3">
-        <v>-1.9</v>
+        <v>8.3557495469716248</v>
       </c>
       <c r="H19" s="3">
-        <v>-2.9892213020444514</v>
+        <v>29.889527562098948</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -11019,22 +11037,22 @@
         <v>7</v>
       </c>
       <c r="C20" s="6">
-        <v>112.47199999999999</v>
+        <v>14556</v>
       </c>
       <c r="D20" s="3">
-        <v>-0.9</v>
+        <v>9.451838484096541</v>
       </c>
       <c r="E20" s="3">
-        <v>-3.8436218728012057</v>
+        <v>34.003400472896217</v>
       </c>
       <c r="F20" s="6">
-        <v>114.69799999999999</v>
+        <v>1567229.72</v>
       </c>
       <c r="G20" s="3">
-        <v>3.5</v>
+        <v>11.865790207112381</v>
       </c>
       <c r="H20" s="3">
-        <v>-3.4633622987749484</v>
+        <v>33.191924836555991</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -11045,22 +11063,22 @@
         <v>8</v>
       </c>
       <c r="C21" s="6">
-        <v>93.984999999999999</v>
+        <v>15254</v>
       </c>
       <c r="D21" s="3">
-        <v>-8.8000000000000007</v>
+        <v>9.0350250178699021</v>
       </c>
       <c r="E21" s="3">
-        <v>-4.6784881598941324</v>
+        <v>37.747097878075834</v>
       </c>
       <c r="F21" s="6">
-        <v>85.929000000000002</v>
+        <v>1661109.79</v>
       </c>
       <c r="G21" s="3">
-        <v>-1</v>
+        <v>10.501794933453045</v>
       </c>
       <c r="H21" s="3">
-        <v>-3.9577589672957942</v>
+        <v>36.6408844058585</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -11071,22 +11089,22 @@
         <v>9</v>
       </c>
       <c r="C22" s="6">
-        <v>111.84399999999999</v>
+        <v>15512</v>
       </c>
       <c r="D22" s="3">
-        <v>-2.7</v>
+        <v>15.977570093457949</v>
       </c>
       <c r="E22" s="3">
-        <v>-5.5352699570385431</v>
+        <v>41.640657991586664</v>
       </c>
       <c r="F22" s="6">
-        <v>106.408</v>
+        <v>1590970.0299999998</v>
       </c>
       <c r="G22" s="3">
-        <v>3</v>
+        <v>11.580245332200413</v>
       </c>
       <c r="H22" s="3">
-        <v>-4.4717417867640448</v>
+        <v>40.230860080331652</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -11097,22 +11115,22 @@
         <v>10</v>
       </c>
       <c r="C23" s="6">
-        <v>121.601</v>
+        <v>16811</v>
       </c>
       <c r="D23" s="3">
-        <v>-0.4</v>
+        <v>16.476131088477786</v>
       </c>
       <c r="E23" s="3">
-        <v>-6.412053294082412</v>
+        <v>45.675698903686758</v>
       </c>
       <c r="F23" s="6">
-        <v>114.613</v>
+        <v>1639199.0100000002</v>
       </c>
       <c r="G23" s="3">
-        <v>0.9</v>
+        <v>14.541820283607754</v>
       </c>
       <c r="H23" s="3">
-        <v>-5.0044358364084713</v>
+        <v>43.954490455753927</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -11123,22 +11141,22 @@
         <v>11</v>
       </c>
       <c r="C24" s="6">
-        <v>113.40900000000001</v>
+        <v>18014</v>
       </c>
       <c r="D24" s="3">
-        <v>-0.3</v>
+        <v>15.786090757166725</v>
       </c>
       <c r="E24" s="3">
-        <v>-7.3067273071266978</v>
+        <v>49.842056545752371</v>
       </c>
       <c r="F24" s="6">
-        <v>108.345</v>
+        <v>1701239.28</v>
       </c>
       <c r="G24" s="3">
-        <v>-0.6</v>
+        <v>12.856274411563007</v>
       </c>
       <c r="H24" s="3">
-        <v>-5.5544473245004315</v>
+        <v>47.802424501879635</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -11149,22 +11167,22 @@
         <v>12</v>
       </c>
       <c r="C25" s="6">
-        <v>93.247</v>
+        <v>18580</v>
       </c>
       <c r="D25" s="3">
-        <v>-12.7</v>
+        <v>13.244346925092954</v>
       </c>
       <c r="E25" s="3">
-        <v>-8.2167636285713801</v>
+        <v>54.127539101394802</v>
       </c>
       <c r="F25" s="6">
-        <v>95.063000000000002</v>
+        <v>1725934.4300000002</v>
       </c>
       <c r="G25" s="3">
-        <v>2.2000000000000002</v>
+        <v>13.219546820826199</v>
       </c>
       <c r="H25" s="3">
-        <v>-6.1199724290448652</v>
+        <v>51.763268641923354</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -11175,22 +11193,22 @@
         <v>1</v>
       </c>
       <c r="C26" s="6">
-        <v>111.078</v>
+        <v>21237</v>
       </c>
       <c r="D26" s="3">
-        <v>-5.3</v>
+        <v>12.890708058685952</v>
       </c>
       <c r="E26" s="3">
-        <v>-9.1391473125312199</v>
+        <v>58.517589756601147</v>
       </c>
       <c r="F26" s="6">
-        <v>102.997</v>
+        <v>1867077.27</v>
       </c>
       <c r="G26" s="3">
-        <v>-4.3</v>
+        <v>12.462479172563889</v>
       </c>
       <c r="H26" s="3">
-        <v>-6.6988632692047325</v>
+        <v>55.823202483121165</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -11201,22 +11219,22 @@
         <v>2</v>
       </c>
       <c r="C27" s="6">
-        <v>104.83199999999999</v>
+        <v>20710.68</v>
       </c>
       <c r="D27" s="3">
-        <v>-9.4</v>
+        <v>12.772556493329713</v>
       </c>
       <c r="E27" s="3">
-        <v>-10.071174748980104</v>
+        <v>62.994812586790701</v>
       </c>
       <c r="F27" s="6">
-        <v>103.758</v>
+        <v>1810993.2600000002</v>
       </c>
       <c r="G27" s="3">
-        <v>-0.4</v>
+        <v>13.224745084416313</v>
       </c>
       <c r="H27" s="3">
-        <v>-7.2883941882798648</v>
+        <v>59.965728985360464</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -11227,22 +11245,22 @@
         <v>3</v>
       </c>
       <c r="C28" s="6">
-        <v>102.211</v>
+        <v>20181</v>
       </c>
       <c r="D28" s="3">
-        <v>-16.100000000000001</v>
+        <v>18.01064265247647</v>
       </c>
       <c r="E28" s="3">
-        <v>-11.009875720439659</v>
+        <v>67.538643133931515</v>
       </c>
       <c r="F28" s="6">
-        <v>96.975999999999999</v>
+        <v>1789266.14</v>
       </c>
       <c r="G28" s="3">
-        <v>-12.1</v>
+        <v>17.545293026686171</v>
       </c>
       <c r="H28" s="3">
-        <v>-7.8856729418430644</v>
+        <v>64.171339947187647</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -11253,22 +11271,22 @@
         <v>4</v>
       </c>
       <c r="C29" s="6">
-        <v>74.177000000000007</v>
+        <v>55776.28</v>
       </c>
       <c r="D29" s="3">
-        <v>-36</v>
+        <v>251.08126140869894</v>
       </c>
       <c r="E29" s="3">
-        <v>-11.952233400073945</v>
+        <v>72.125029283318483</v>
       </c>
       <c r="F29" s="6">
-        <v>67.994</v>
+        <v>4938729.3099999996</v>
       </c>
       <c r="G29" s="3">
-        <v>-34.1</v>
+        <v>236.23041153923779</v>
       </c>
       <c r="H29" s="3">
-        <v>-8.4873289247596144</v>
+        <v>68.417281265489322</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -11279,22 +11297,22 @@
         <v>5</v>
       </c>
       <c r="C30" s="6">
-        <v>87.876999999999995</v>
+        <v>62661</v>
       </c>
       <c r="D30" s="3">
-        <v>-27.2</v>
+        <v>293.64869958537503</v>
       </c>
       <c r="E30" s="3">
-        <v>-12.895584441899766</v>
+        <v>76.726479475768613</v>
       </c>
       <c r="F30" s="6">
-        <v>82.668000000000006</v>
+        <v>5526120</v>
       </c>
       <c r="G30" s="3">
-        <v>-27.8</v>
+        <v>279.1495623967383</v>
       </c>
       <c r="H30" s="3">
-        <v>-9.0902841934960605</v>
+        <v>72.677560917227069</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -11553,8 +11571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -11578,22 +11596,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -13941,8 +13959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -13966,22 +13984,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -15019,22 +15037,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -16173,8 +16191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -16198,22 +16216,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>133</v>
+        <v>205</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>135</v>
+        <v>207</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>136</v>
+        <v>208</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>137</v>
+        <v>209</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>138</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -16230,7 +16248,7 @@
         <v>21.917808219178081</v>
       </c>
       <c r="E2" s="3">
-        <v>-5.4632902470841387</v>
+        <v>-5.3546917291190583</v>
       </c>
       <c r="F2" s="4">
         <v>9403</v>
@@ -16239,7 +16257,7 @@
         <v>5.7824277196534934</v>
       </c>
       <c r="H2" s="3">
-        <v>-0.91109167614868991</v>
+        <v>-0.72080295359944624</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -16256,7 +16274,7 @@
         <v>-6.944444444444442</v>
       </c>
       <c r="E3" s="3">
-        <v>-5.8070464357588376</v>
+        <v>-5.7225114845167298</v>
       </c>
       <c r="F3" s="4">
         <v>8738</v>
@@ -16265,7 +16283,7 @@
         <v>-1.1985526910900046</v>
       </c>
       <c r="H3" s="3">
-        <v>-1.065848063285912</v>
+        <v>-0.91761609239784581</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -16282,7 +16300,7 @@
         <v>-25.757575757575758</v>
       </c>
       <c r="E4" s="3">
-        <v>-6.1379322573137465</v>
+        <v>-6.0815295663343241</v>
       </c>
       <c r="F4" s="4">
         <v>9265</v>
@@ -16291,7 +16309,7 @@
         <v>-12.138454243717401</v>
       </c>
       <c r="H4" s="3">
-        <v>-1.2325848099355603</v>
+        <v>-1.1335249533510001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -16308,7 +16326,7 @@
         <v>5.0000000000000044</v>
       </c>
       <c r="E5" s="3">
-        <v>-6.4601958026295296</v>
+        <v>-6.4363048805668761</v>
       </c>
       <c r="F5" s="4">
         <v>8817</v>
@@ -16317,7 +16335,7 @@
         <v>13.212634822804304</v>
       </c>
       <c r="H5" s="3">
-        <v>-1.4140808278047852</v>
+        <v>-1.3718522308170213</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -16334,7 +16352,7 @@
         <v>-12.5</v>
       </c>
       <c r="E6" s="3">
-        <v>-6.7794476378299251</v>
+        <v>-6.7927627253060354</v>
       </c>
       <c r="F6" s="4">
         <v>8830</v>
@@ -16343,7 +16361,7 @@
         <v>0.50079672205782799</v>
       </c>
       <c r="H6" s="3">
-        <v>-1.6138723806447495</v>
+        <v>-1.6366848503547418</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -16360,7 +16378,7 @@
         <v>-26.470588235294112</v>
       </c>
       <c r="E7" s="3">
-        <v>-7.1005024821079328</v>
+        <v>-7.1560342108045232</v>
       </c>
       <c r="F7" s="4">
         <v>8120</v>
@@ -16369,7 +16387,7 @@
         <v>-2.5093048385160244</v>
       </c>
       <c r="H7" s="3">
-        <v>-1.8344799880642131</v>
+        <v>-1.9310969259220478</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -16386,7 +16404,7 @@
         <v>-5.6603773584905648</v>
       </c>
       <c r="E8" s="3">
-        <v>-7.4285723152372602</v>
+        <v>-7.5316467832369147</v>
       </c>
       <c r="F8" s="4">
         <v>7695</v>
@@ -16395,7 +16413,7 @@
         <v>3.4969737726967098</v>
       </c>
       <c r="H8" s="3">
-        <v>-2.0782773176509153</v>
+        <v>-2.2580141352565199</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -16412,7 +16430,7 @@
         <v>38.46153846153846</v>
       </c>
       <c r="E9" s="3">
-        <v>-7.7702142618355863</v>
+        <v>-7.9264691772517102</v>
       </c>
       <c r="F9" s="4">
         <v>5870</v>
@@ -16421,7 +16439,7 @@
         <v>-0.67681895093062439</v>
       </c>
       <c r="H9" s="3">
-        <v>-2.347684899829432</v>
+        <v>-2.6204023094230018</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -16438,7 +16456,7 @@
         <v>-25</v>
       </c>
       <c r="E10" s="3">
-        <v>-8.1318626552041504</v>
+        <v>-8.347240178231802</v>
       </c>
       <c r="F10" s="4">
         <v>5882</v>
@@ -16447,7 +16465,7 @@
         <v>-4.4664609387688792</v>
       </c>
       <c r="H10" s="3">
-        <v>-2.6447360948097312</v>
+        <v>-3.0208276275482846</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -16464,7 +16482,7 @@
         <v>8.0645161290322509</v>
       </c>
       <c r="E11" s="3">
-        <v>-8.5167412902606241</v>
+        <v>-8.7974771821407227</v>
       </c>
       <c r="F11" s="4">
         <v>7723</v>
@@ -16473,7 +16491,7 @@
         <v>6.7302377003869651</v>
       </c>
       <c r="H11" s="3">
-        <v>-2.9713482304442187</v>
+        <v>-3.461721297692598</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -16490,7 +16508,7 @@
         <v>12.307692307692308</v>
       </c>
       <c r="E12" s="3">
-        <v>-8.9292453603494017</v>
+        <v>-9.2818540265962959</v>
       </c>
       <c r="F12" s="4">
         <v>7969</v>
@@ -16499,7 +16517,7 @@
         <v>3.2789009849663042</v>
       </c>
       <c r="H12" s="3">
-        <v>-3.3295651432550204</v>
+        <v>-3.9456149191183396</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -16516,7 +16534,7 @@
         <v>22.916666666666675</v>
       </c>
       <c r="E13" s="3">
-        <v>-9.3726185826052077</v>
+        <v>-9.8038735774586243</v>
       </c>
       <c r="F13" s="4">
         <v>6809</v>
@@ -16525,7 +16543,7 @@
         <v>1.0987379361544258</v>
       </c>
       <c r="H13" s="3">
-        <v>-3.7207569485190648</v>
+        <v>-4.4743323161574846</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -16542,7 +16560,7 @@
         <v>-4.4943820224719104</v>
       </c>
       <c r="E14" s="3">
-        <v>-9.8486298868247069</v>
+        <v>-10.365539426536822</v>
       </c>
       <c r="F14" s="4">
         <v>8995</v>
@@ -16551,7 +16569,7 @@
         <v>-4.3390407316813757</v>
       </c>
       <c r="H14" s="3">
-        <v>-4.1458348402543761</v>
+        <v>-5.0491956106486686</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -16568,7 +16586,7 @@
         <v>-17.910447761194025</v>
       </c>
       <c r="E15" s="3">
-        <v>-10.356805891328918</v>
+        <v>-10.966582905900824</v>
       </c>
       <c r="F15" s="4">
         <v>9382</v>
@@ -16577,7 +16595,7 @@
         <v>7.3701075761043677</v>
       </c>
       <c r="H15" s="3">
-        <v>-4.6053753253342089</v>
+        <v>-5.6711399056630052</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -16594,7 +16612,7 @@
         <v>28.57142857142858</v>
       </c>
       <c r="E16" s="3">
-        <v>-10.896301391670505</v>
+        <v>-11.606327628356395</v>
       </c>
       <c r="F16" s="4">
         <v>9437</v>
@@ -16603,7 +16621,7 @@
         <v>1.8564490016189872</v>
       </c>
       <c r="H16" s="3">
-        <v>-5.0999683277076109</v>
+        <v>-6.3410509879605677</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -16620,7 +16638,7 @@
         <v>-34.523809523809526</v>
       </c>
       <c r="E17" s="3">
-        <v>-11.466795741865317</v>
+        <v>-12.284579419546475</v>
       </c>
       <c r="F17" s="4">
         <v>8683</v>
@@ -16629,7 +16647,7 @@
         <v>-1.5197913122377171</v>
       </c>
       <c r="H17" s="3">
-        <v>-5.6293721405665851</v>
+        <v>-7.058909002115195</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -16646,16 +16664,16 @@
         <v>-28.571428571428569</v>
       </c>
       <c r="E18" s="3">
-        <v>-12.06522748134843</v>
+        <v>-12.998353983155683</v>
       </c>
       <c r="F18" s="4">
-        <v>8583</v>
+        <v>8585</v>
       </c>
       <c r="G18" s="3">
-        <v>-2.7972819932049808</v>
+        <v>-2.7746319365798411</v>
       </c>
       <c r="H18" s="3">
-        <v>-6.1928619725663747</v>
+        <v>-7.8241248218681161</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -16672,7 +16690,7 @@
         <v>26</v>
       </c>
       <c r="E19" s="3">
-        <v>-12.690136331067556</v>
+        <v>-13.746211413848103</v>
       </c>
       <c r="F19" s="4">
         <v>7433</v>
@@ -16681,7 +16699,7 @@
         <v>-8.4605911330049253</v>
       </c>
       <c r="H19" s="3">
-        <v>-6.7894276448047002</v>
+        <v>-8.6357246600098723</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -16698,7 +16716,7 @@
         <v>-9.9999999999999982</v>
       </c>
       <c r="E20" s="3">
-        <v>-13.341208275934997</v>
+        <v>-14.527793269800892</v>
       </c>
       <c r="F20" s="4">
         <v>7820</v>
@@ -16707,7 +16725,7 @@
         <v>1.6244314489928469</v>
       </c>
       <c r="H20" s="3">
-        <v>-7.417823174214047</v>
+        <v>-9.4923840701028599</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -16724,7 +16742,7 @@
         <v>-42.592592592592595</v>
       </c>
       <c r="E21" s="3">
-        <v>-14.015442485840063</v>
+        <v>-15.339980955620799</v>
       </c>
       <c r="F21" s="4">
         <v>5366</v>
@@ -16733,7 +16751,7 @@
         <v>-8.5860306643952278</v>
       </c>
       <c r="H21" s="3">
-        <v>-8.0769186307469134</v>
+        <v>-10.392766443658987</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -16750,7 +16768,7 @@
         <v>42.857142857142861</v>
       </c>
       <c r="E22" s="3">
-        <v>-14.709606102319567</v>
+        <v>-16.179341445826395</v>
       </c>
       <c r="F22" s="4">
         <v>5787</v>
@@ -16759,7 +16777,7 @@
         <v>-1.6150969058143505</v>
       </c>
       <c r="H22" s="3">
-        <v>-8.764956150006963</v>
+        <v>-11.334763171112444</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -16776,7 +16794,7 @@
         <v>-20.895522388059707</v>
       </c>
       <c r="E23" s="3">
-        <v>-15.422450791223293</v>
+        <v>-17.044334257411041</v>
       </c>
       <c r="F23" s="4">
         <v>8029</v>
@@ -16785,7 +16803,7 @@
         <v>3.9621908584746901</v>
       </c>
       <c r="H23" s="3">
-        <v>-9.4802132226001987</v>
+        <v>-12.316140175134976</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -16802,7 +16820,7 @@
         <v>-49.315068493150683</v>
       </c>
       <c r="E24" s="3">
-        <v>-16.148730527501058</v>
+        <v>-17.92931915151372</v>
       </c>
       <c r="F24" s="4">
         <v>7331</v>
@@ -16811,7 +16829,7 @@
         <v>-8.0060233404442229</v>
       </c>
       <c r="H24" s="3">
-        <v>-10.220470821129553</v>
+        <v>-13.333988401574349</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -16828,7 +16846,7 @@
         <v>-23.728813559322038</v>
       </c>
       <c r="E25" s="3">
-        <v>-16.883579360519132</v>
+        <v>-18.828923332893606</v>
       </c>
       <c r="F25" s="4">
         <v>7097</v>
@@ -16837,7 +16855,7 @@
         <v>4.2296959906006792</v>
       </c>
       <c r="H25" s="3">
-        <v>-10.982576417914551</v>
+        <v>-14.384268356623219</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -16854,7 +16872,7 @@
         <v>-42.352941176470594</v>
       </c>
       <c r="E26" s="3">
-        <v>-17.624434557558065</v>
+        <v>-19.73995357223637</v>
       </c>
       <c r="F26" s="4">
         <v>8656</v>
@@ -16863,7 +16881,7 @@
         <v>-3.7687604224569182</v>
       </c>
       <c r="H26" s="3">
-        <v>-11.763223704199671</v>
+        <v>-15.462570548900549</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -16880,7 +16898,7 @@
         <v>1.8181818181818077</v>
       </c>
       <c r="E27" s="3">
-        <v>-18.36920874938443</v>
+        <v>-20.6595569103823</v>
       </c>
       <c r="F27" s="4">
         <v>8516</v>
@@ -16889,7 +16907,7 @@
         <v>-9.2304412705180088</v>
       </c>
       <c r="H27" s="3">
-        <v>-12.558049963423242</v>
+        <v>-16.5631928506123</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -16906,7 +16924,7 @@
         <v>-19.047619047619047</v>
       </c>
       <c r="E28" s="3">
-        <v>-19.117531824168896</v>
+        <v>-21.586450734533084</v>
       </c>
       <c r="F28" s="4">
         <v>6767</v>
@@ -16915,7 +16933,7 @@
         <v>-28.292889689519974</v>
       </c>
       <c r="H28" s="3">
-        <v>-13.36213730796236</v>
+        <v>-17.679621063816761</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -16932,7 +16950,7 @@
         <v>-45.45454545454546</v>
       </c>
       <c r="E29" s="3">
-        <v>-19.867631767959374</v>
+        <v>-22.517791477812036</v>
       </c>
       <c r="F29" s="4">
         <v>2311</v>
@@ -16941,16 +16959,34 @@
         <v>-73.38477484740298</v>
       </c>
       <c r="H29" s="3">
-        <v>-14.170336766257114</v>
+        <v>-18.804831771712493</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="A30" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="4">
+        <v>28</v>
+      </c>
+      <c r="D30" s="3">
+        <v>-43.999999999999993</v>
+      </c>
+      <c r="E30" s="3">
+        <v>-23.450559265586435</v>
+      </c>
+      <c r="F30" s="4">
+        <v>3788</v>
+      </c>
+      <c r="G30" s="3">
+        <v>-55.876528829353525</v>
+      </c>
+      <c r="H30" s="3">
+        <v>-19.93253859004151</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C31" s="4"/>
@@ -17367,8 +17403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection sqref="A1:H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -17392,22 +17428,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>133</v>
+        <v>205</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>135</v>
+        <v>207</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>136</v>
+        <v>208</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>137</v>
+        <v>209</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>138</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -17424,7 +17460,7 @@
         <v>-13.461538461538458</v>
       </c>
       <c r="E2" s="3">
-        <v>14.325001356728423</v>
+        <v>14.874109722333408</v>
       </c>
       <c r="F2" s="4">
         <v>3710</v>
@@ -17433,7 +17469,7 @@
         <v>6.9780853517877661</v>
       </c>
       <c r="H2" s="3">
-        <v>2.3277354577584437</v>
+        <v>2.6067104698303343</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -17450,7 +17486,7 @@
         <v>10.000000000000009</v>
       </c>
       <c r="E3" s="3">
-        <v>14.574862459457627</v>
+        <v>15.002297840555617</v>
       </c>
       <c r="F3" s="4">
         <v>2291</v>
@@ -17459,7 +17495,7 @@
         <v>1.9581664441477464</v>
       </c>
       <c r="H3" s="3">
-        <v>2.3162146740900011</v>
+        <v>2.5339993534950316</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -17476,7 +17512,7 @@
         <v>8.333333333333325</v>
       </c>
       <c r="E4" s="3">
-        <v>14.877530197413595</v>
+        <v>15.162719995947089</v>
       </c>
       <c r="F4" s="4">
         <v>1756</v>
@@ -17485,7 +17521,7 @@
         <v>-11.803114013058769</v>
       </c>
       <c r="H4" s="3">
-        <v>2.2811136956199536</v>
+        <v>2.4273367676888689</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -17502,7 +17538,7 @@
         <v>39.999999999999993</v>
       </c>
       <c r="E5" s="3">
-        <v>15.233051495135578</v>
+        <v>15.353851533778268</v>
       </c>
       <c r="F5" s="4">
         <v>1486</v>
@@ -17511,7 +17547,7 @@
         <v>12.832194381169316</v>
       </c>
       <c r="H5" s="3">
-        <v>2.2205136852274583</v>
+        <v>2.2840102758161009</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -17528,7 +17564,7 @@
         <v>-31.999999999999996</v>
       </c>
       <c r="E6" s="3">
-        <v>15.641018819047268</v>
+        <v>15.573693536356917</v>
       </c>
       <c r="F6" s="4">
         <v>1524</v>
@@ -17537,7 +17573,7 @@
         <v>0.92715231788078611</v>
       </c>
       <c r="H6" s="3">
-        <v>2.1315177344230145</v>
+        <v>2.1003192155323203</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -17554,7 +17590,7 @@
         <v>16.666666666666675</v>
       </c>
       <c r="E7" s="3">
-        <v>16.102744562551862</v>
+        <v>15.82195862407873</v>
       </c>
       <c r="F7" s="4">
         <v>1370</v>
@@ -17563,7 +17599,7 @@
         <v>-4.2627533193570937</v>
       </c>
       <c r="H7" s="3">
-        <v>2.0119658569876733</v>
+        <v>1.8732954372782138</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -17580,7 +17616,7 @@
         <v>-70</v>
       </c>
       <c r="E8" s="3">
-        <v>16.616232714967904</v>
+        <v>16.095055688621603</v>
       </c>
       <c r="F8" s="4">
         <v>1485</v>
@@ -17589,7 +17625,7 @@
         <v>8.3150984682713425</v>
       </c>
       <c r="H8" s="3">
-        <v>1.8596144302152262</v>
+        <v>1.5998893215710206</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -17606,7 +17642,7 @@
         <v>110.00000000000001</v>
       </c>
       <c r="E9" s="3">
-        <v>17.179526426871167</v>
+        <v>16.389452281944166</v>
       </c>
       <c r="F9" s="4">
         <v>1357</v>
@@ -17615,7 +17651,7 @@
         <v>10.504885993485335</v>
       </c>
       <c r="H9" s="3">
-        <v>1.6717840870122187</v>
+        <v>1.2766251344309907</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -17632,7 +17668,7 @@
         <v>-70.588235294117638</v>
       </c>
       <c r="E10" s="3">
-        <v>17.784653832676664</v>
+        <v>16.695637132693342</v>
       </c>
       <c r="F10" s="4">
         <v>1104</v>
@@ -17641,7 +17677,7 @@
         <v>-0.54054054054053502</v>
       </c>
       <c r="H10" s="3">
-        <v>1.4462437577878382</v>
+        <v>0.9004934758468951</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -17658,7 +17694,7 @@
         <v>-17.647058823529417</v>
       </c>
       <c r="E11" s="3">
-        <v>18.430088933019768</v>
+        <v>17.010599701996476</v>
       </c>
       <c r="F11" s="4">
         <v>1665</v>
@@ -17667,7 +17703,7 @@
         <v>10.484406104844069</v>
       </c>
       <c r="H11" s="3">
-        <v>1.1813757828058888</v>
+        <v>0.46912579725605014</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -17684,7 +17720,7 @@
         <v>83.333333333333329</v>
       </c>
       <c r="E12" s="3">
-        <v>19.108168722346491</v>
+        <v>17.325268070951275</v>
       </c>
       <c r="F12" s="4">
         <v>1992</v>
@@ -17693,7 +17729,7 @@
         <v>10.055248618784528</v>
       </c>
       <c r="H12" s="3">
-        <v>0.87542453119834629</v>
+        <v>-1.9946521710921275E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -17710,7 +17746,7 @@
         <v>63.636363636363647</v>
       </c>
       <c r="E13" s="3">
-        <v>19.808724837619756</v>
+        <v>17.628163538813396</v>
       </c>
       <c r="F13" s="4">
         <v>2647</v>
@@ -17719,7 +17755,7 @@
         <v>1.9252984212552837</v>
       </c>
       <c r="H13" s="3">
-        <v>0.52728041586954999</v>
+        <v>-0.5684965958464806</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -17736,7 +17772,7 @@
         <v>-13.33333333333333</v>
       </c>
       <c r="E14" s="3">
-        <v>20.526048996678249</v>
+        <v>17.9123912982595</v>
       </c>
       <c r="F14" s="4">
         <v>4157</v>
@@ -17745,7 +17781,7 @@
         <v>12.048517520215629</v>
       </c>
       <c r="H14" s="3">
-        <v>0.1364713375076993</v>
+        <v>-1.1775978736138881</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -17762,7 +17798,7 @@
         <v>-27.27272727272727</v>
       </c>
       <c r="E15" s="3">
-        <v>21.257476503388339</v>
+        <v>18.174251555861904</v>
       </c>
       <c r="F15" s="4">
         <v>2311</v>
@@ -17771,7 +17807,7 @@
         <v>0.87298123090353563</v>
       </c>
       <c r="H15" s="3">
-        <v>-0.29737771861529905</v>
+        <v>-1.848150623266883</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -17788,7 +17824,7 @@
         <v>-30.76923076923077</v>
       </c>
       <c r="E16" s="3">
-        <v>21.997991315621267</v>
+        <v>18.407874676204624</v>
       </c>
       <c r="F16" s="4">
         <v>1855</v>
@@ -17797,7 +17833,7 @@
         <v>5.6378132118451108</v>
       </c>
       <c r="H16" s="3">
-        <v>-0.77381454179818354</v>
+        <v>-2.5801366328235216</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -17814,7 +17850,7 @@
         <v>-9.5238095238095237</v>
       </c>
       <c r="E17" s="3">
-        <v>22.739207238208259</v>
+        <v>18.604234983675248</v>
       </c>
       <c r="F17" s="4">
         <v>1610</v>
@@ -17823,7 +17859,7 @@
         <v>8.3445491251682427</v>
       </c>
       <c r="H17" s="3">
-        <v>-1.2923056464126428</v>
+        <v>-3.3733487228119872</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -17840,16 +17876,16 @@
         <v>11.764705882352944</v>
       </c>
       <c r="E18" s="3">
-        <v>23.46907368555798</v>
+        <v>18.750891725894313</v>
       </c>
       <c r="F18" s="4">
-        <v>1629</v>
+        <v>1631</v>
       </c>
       <c r="G18" s="3">
-        <v>6.889763779527569</v>
+        <v>7.0209973753280863</v>
       </c>
       <c r="H18" s="3">
-        <v>-1.8518722949030288</v>
+        <v>-4.2270090227990273</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -17866,7 +17902,7 @@
         <v>-7.1428571428571397</v>
       </c>
       <c r="E19" s="3">
-        <v>24.17329958480396</v>
+        <v>18.833450814058232</v>
       </c>
       <c r="F19" s="4">
         <v>1255</v>
@@ -17875,7 +17911,7 @@
         <v>-8.394160583941602</v>
       </c>
       <c r="H19" s="3">
-        <v>-2.4508665236878895</v>
+        <v>-5.1395259194452798</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -17892,7 +17928,7 @@
         <v>200</v>
       </c>
       <c r="E20" s="3">
-        <v>24.83678105976006</v>
+        <v>18.837033007568724</v>
       </c>
       <c r="F20" s="4">
         <v>1622</v>
@@ -17901,7 +17937,7 @@
         <v>9.2255892255892249</v>
       </c>
       <c r="H20" s="3">
-        <v>-3.0870333111250479</v>
+        <v>-6.1085266878559565</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -17918,7 +17954,7 @@
         <v>-52.380952380952387</v>
       </c>
       <c r="E21" s="3">
-        <v>25.442239501134054</v>
+        <v>18.744955155552727</v>
       </c>
       <c r="F21" s="4">
         <v>1164</v>
@@ -17927,7 +17963,7 @@
         <v>-14.222549742078117</v>
       </c>
       <c r="H21" s="3">
-        <v>-3.7585303643265111</v>
+        <v>-7.1318646194324131</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -17944,7 +17980,7 @@
         <v>400</v>
       </c>
       <c r="E22" s="3">
-        <v>25.984560412060119</v>
+        <v>18.553114868733868</v>
       </c>
       <c r="F22" s="4">
         <v>1254</v>
@@ -17953,7 +17989,7 @@
         <v>13.586956521739136</v>
       </c>
       <c r="H22" s="3">
-        <v>-4.4626603471725694</v>
+        <v>-8.2063281364153493</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -17970,7 +18006,7 @@
         <v>7.1428571428571397</v>
       </c>
       <c r="E23" s="3">
-        <v>26.453224907347291</v>
+        <v>18.2524704587013</v>
       </c>
       <c r="F23" s="4">
         <v>1743</v>
@@ -17979,7 +18015,7 @@
         <v>4.6846846846846812</v>
       </c>
       <c r="H23" s="3">
-        <v>-5.1974525915558578</v>
+        <v>-9.329198069734538</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -17996,7 +18032,7 @@
         <v>9.0909090909090828</v>
       </c>
       <c r="E24" s="3">
-        <v>26.863687396220428</v>
+        <v>17.860469604067177</v>
       </c>
       <c r="F24" s="4">
         <v>1982</v>
@@ -18005,7 +18041,7 @@
         <v>-0.5020080321285092</v>
       </c>
       <c r="H24" s="3">
-        <v>-5.9596829837531144</v>
+        <v>-10.496241827774048</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -18022,7 +18058,7 @@
         <v>-38.888888888888886</v>
       </c>
       <c r="E25" s="3">
-        <v>27.230061290142967</v>
+        <v>17.393788482518939</v>
       </c>
       <c r="F25" s="4">
         <v>2713</v>
@@ -18031,7 +18067,7 @@
         <v>2.4933887419720469</v>
       </c>
       <c r="H25" s="3">
-        <v>-6.7454411505080056</v>
+        <v>-11.702253632615559</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -18048,7 +18084,7 @@
         <v>23.076923076923084</v>
       </c>
       <c r="E26" s="3">
-        <v>27.565225779862704</v>
+        <v>16.868494274486174</v>
       </c>
       <c r="F26" s="4">
         <v>3553</v>
@@ -18057,7 +18093,7 @@
         <v>-14.52970892470532</v>
       </c>
       <c r="H26" s="3">
-        <v>-7.5504377133592229</v>
+        <v>-12.94133366232716</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -18074,7 +18110,7 @@
         <v>20.833333333333325</v>
       </c>
       <c r="E27" s="3">
-        <v>27.877468462365002</v>
+        <v>16.296745641136564</v>
       </c>
       <c r="F27" s="4">
         <v>2416</v>
@@ -18083,7 +18119,7 @@
         <v>4.543487667676338</v>
       </c>
       <c r="H27" s="3">
-        <v>-8.3697417084362566</v>
+        <v>-14.206596286478707</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -18100,7 +18136,7 @@
         <v>27.777777777777768</v>
       </c>
       <c r="E28" s="3">
-        <v>28.174765246947509</v>
+        <v>15.691132384526846</v>
       </c>
       <c r="F28" s="4">
         <v>1464</v>
@@ -18109,7 +18145,7 @@
         <v>-21.078167115902968</v>
       </c>
       <c r="H28" s="3">
-        <v>-9.198906843480497</v>
+        <v>-15.491266178477717</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -18126,7 +18162,7 @@
         <v>-78.94736842105263</v>
       </c>
       <c r="E29" s="3">
-        <v>28.464602866857245</v>
+        <v>15.064559347525714</v>
       </c>
       <c r="F29" s="4">
         <v>401</v>
@@ -18135,16 +18171,34 @@
         <v>-75.093167701863351</v>
       </c>
       <c r="H29" s="3">
-        <v>-10.032590074193326</v>
+        <v>-16.787265922568228</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="A30" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="4">
+        <v>2</v>
+      </c>
+      <c r="D30" s="3">
+        <v>-89.473684210526315</v>
+      </c>
+      <c r="E30" s="3">
+        <v>14.430770723376394</v>
+      </c>
+      <c r="F30" s="4">
+        <v>481</v>
+      </c>
+      <c r="G30" s="3">
+        <v>-70.508890251379512</v>
+      </c>
+      <c r="H30" s="3">
+        <v>-18.08690608222604</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C31" s="4"/>
@@ -18517,22 +18571,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -19588,22 +19642,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -20677,22 +20731,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -21694,22 +21748,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -22855,22 +22909,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -24034,22 +24088,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -26217,22 +26271,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -28502,22 +28556,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -29573,22 +29627,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -30654,22 +30708,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -31887,22 +31941,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -33119,22 +33173,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update monthly data of 'pernoctaciones_hoteleras'
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_mensual.xlsx
+++ b/etl/data/input/Datos_carga_mensual.xlsx
@@ -4198,10 +4198,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4257,7 +4257,7 @@
         <v>7.7448234118326</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>6.83499133306905</v>
+        <v>7.16844606008051</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>15395882</v>
@@ -4266,7 +4266,7 @@
         <v>1.28409960337328</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>3.44548862213621</v>
+        <v>3.8001529135162</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4283,7 +4283,7 @@
         <v>-3.25488514824677</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>6.41790852853539</v>
+        <v>6.6997736450367</v>
       </c>
       <c r="F3" s="4" t="n">
         <v>16527859</v>
@@ -4292,7 +4292,7 @@
         <v>1.10925655554872</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>3.01630956705894</v>
+        <v>3.31571043337636</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4309,7 +4309,7 @@
         <v>25.8205265319724</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>5.95991495615601</v>
+        <v>6.18057306455911</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>21918931</v>
@@ -4318,7 +4318,7 @@
         <v>6.87656485868566</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>2.55008137888517</v>
+        <v>2.78393909313009</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4335,7 +4335,7 @@
         <v>-13.7959787998227</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>5.45805143937161</v>
+        <v>5.6071034237794</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>25207350</v>
@@ -4344,7 +4344,7 @@
         <v>-8.50136042761834</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>2.04431807875257</v>
+        <v>2.20151843549437</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4361,7 +4361,7 @@
         <v>1.63975494773281</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>4.91073801076012</v>
+        <v>4.97698771348666</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>31921157</v>
@@ -4370,7 +4370,7 @@
         <v>1.53065593042221</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>1.49683413804048</v>
+        <v>1.56541221330878</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4387,7 +4387,7 @@
         <v>0.0544864650667387</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>4.31505761746618</v>
+        <v>4.28650148820444</v>
       </c>
       <c r="F7" s="4" t="n">
         <v>36168465</v>
@@ -4396,7 +4396,7 @@
         <v>-1.30418533311947</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>0.904711689343023</v>
+        <v>0.871840923936306</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4413,7 +4413,7 @@
         <v>0.119081131561183</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>3.66786605503285</v>
+        <v>3.53168855018091</v>
       </c>
       <c r="F8" s="4" t="n">
         <v>42717096</v>
@@ -4422,7 +4422,7 @@
         <v>-2.07994546912568</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>0.265035213989955</v>
+        <v>0.117022651109181</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4439,7 +4439,7 @@
         <v>7.41865702601789</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>2.96572324600647</v>
+        <v>2.70829881173209</v>
       </c>
       <c r="F9" s="4" t="n">
         <v>46306240</v>
@@ -4448,7 +4448,7 @@
         <v>-0.752182080758534</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>-0.425264202315553</v>
+        <v>-0.70297563437489</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4465,7 +4465,7 @@
         <v>8.42543401220863</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>2.20494266953594</v>
+        <v>1.81184519854767</v>
       </c>
       <c r="F10" s="4" t="n">
         <v>37768667</v>
@@ -4474,7 +4474,7 @@
         <v>-0.508229382013126</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>-1.1694183197511</v>
+        <v>-1.59223952894877</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4491,7 +4491,7 @@
         <v>0.962898487650965</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>1.38214703628265</v>
+        <v>0.838167744526693</v>
       </c>
       <c r="F11" s="4" t="n">
         <v>31132356</v>
@@ -4500,7 +4500,7 @@
         <v>0.756470750778271</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>-1.97068160112472</v>
+        <v>-2.55485804615965</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4517,7 +4517,7 @@
         <v>14.5340745316039</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>0.494391035473448</v>
+        <v>-0.216434239430853</v>
       </c>
       <c r="F12" s="4" t="n">
         <v>18261076</v>
@@ -4526,7 +4526,7 @@
         <v>4.12625882141495</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>-2.83226259334602</v>
+        <v>-3.5948449210723</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4543,7 +4543,7 @@
         <v>6.04826927946704</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>-0.461299758147353</v>
+        <v>-1.35565278056782</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>16655848</v>
@@ -4552,7 +4552,7 @@
         <v>2.73904826972009</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>-3.75718045774458</v>
+        <v>-4.71598393536281</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4569,7 +4569,7 @@
         <v>-0.597050024169421</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>-1.48692479181488</v>
+        <v>-2.5821555652402</v>
       </c>
       <c r="F14" s="4" t="n">
         <v>15506154</v>
@@ -4578,7 +4578,7 @@
         <v>0.716243473417122</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>-4.74797112499619</v>
+        <v>-5.92152268294738</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4595,7 +4595,7 @@
         <v>12.3030635211251</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>-2.58403145935886</v>
+        <v>-3.89809611854978</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>16589486</v>
@@ -4604,7 +4604,7 @@
         <v>0.372867411320477</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>-5.8067193987817</v>
+        <v>-7.21419104717242</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4621,7 +4621,7 @@
         <v>-8.35602094240838</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>-3.75410535775018</v>
+        <v>-5.30549011104692</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>21520914</v>
@@ -4630,7 +4630,7 @@
         <v>-1.81585954169025</v>
       </c>
       <c r="H16" s="3" t="n">
-        <v>-6.93513062343481</v>
+        <v>-8.59625795540122</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4647,7 +4647,7 @@
         <v>15.5324871419808</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>-4.99759825791939</v>
+        <v>-6.80522813275142</v>
       </c>
       <c r="F17" s="4" t="n">
         <v>26808982</v>
@@ -4656,7 +4656,7 @@
         <v>6.35382933945854</v>
       </c>
       <c r="H17" s="3" t="n">
-        <v>-8.13448100531632</v>
+        <v>-10.0694654559375</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4673,7 +4673,7 @@
         <v>4.4948351968451</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>-6.3152815082682</v>
+        <v>-8.39841261610195</v>
       </c>
       <c r="F18" s="4" t="n">
         <v>31905788</v>
@@ -4682,7 +4682,7 @@
         <v>-0.0481467510717093</v>
       </c>
       <c r="H18" s="3" t="n">
-        <v>-9.40569124585079</v>
+        <v>-11.635084736084</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4693,22 +4693,22 @@
         <v>6</v>
       </c>
       <c r="C19" s="4" t="n">
-        <v>292349</v>
+        <v>293090</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>3.37915012040608</v>
+        <v>3.64117923710983</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>-7.70650075682334</v>
+        <v>-10.0845947633097</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>37102583</v>
+        <v>37163185</v>
       </c>
       <c r="G19" s="3" t="n">
-        <v>2.58268632633427</v>
+        <v>2.75024112856324</v>
       </c>
       <c r="H19" s="3" t="n">
-        <v>-10.7486759137999</v>
+        <v>-13.2932464765605</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4725,7 +4725,7 @@
         <v>0.0365967683268353</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>-9.16985094906256</v>
+        <v>-11.8624304121546</v>
       </c>
       <c r="F20" s="4" t="n">
         <v>43205627</v>
@@ -4734,7 +4734,7 @@
         <v>1.14364281691808</v>
       </c>
       <c r="H20" s="3" t="n">
-        <v>-12.1626997484467</v>
+        <v>-15.0432767096154</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4751,7 +4751,7 @@
         <v>-2.46589608132526</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>-10.7031571935972</v>
+        <v>-13.7296222216662</v>
       </c>
       <c r="F21" s="4" t="n">
         <v>46998612</v>
@@ -4760,7 +4760,7 @@
         <v>1.4952023744532</v>
       </c>
       <c r="H21" s="3" t="n">
-        <v>-13.6461017000295</v>
+        <v>-16.8833873364137</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4777,7 +4777,7 @@
         <v>2.72884913753764</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>-12.3036052623913</v>
+        <v>-15.6830465295424</v>
       </c>
       <c r="F22" s="4" t="n">
         <v>37551418</v>
@@ -4786,7 +4786,7 @@
         <v>-0.575209604299776</v>
       </c>
       <c r="H22" s="3" t="n">
-        <v>-15.1962966672199</v>
+        <v>-18.8106661664865</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4803,7 +4803,7 @@
         <v>-2.1503147964703</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>-13.9678088953877</v>
+        <v>-17.7187974702768</v>
       </c>
       <c r="F23" s="4" t="n">
         <v>30508159</v>
@@ -4812,7 +4812,7 @@
         <v>-2.00497835756471</v>
       </c>
       <c r="H23" s="3" t="n">
-        <v>-16.8096480692395</v>
+        <v>-20.8209247184126</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4829,7 +4829,7 @@
         <v>2.05287870398998</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>-15.6913379120843</v>
+        <v>-19.8316905744971</v>
       </c>
       <c r="F24" s="4" t="n">
         <v>18345499</v>
@@ -4838,7 +4838,7 @@
         <v>0.462311202253352</v>
       </c>
       <c r="H24" s="3" t="n">
-        <v>-18.481503972042</v>
+        <v>-22.9087081596208</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4855,7 +4855,7 @@
         <v>5.236765732339</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>-17.4689414726668</v>
+        <v>-22.0154602282012</v>
       </c>
       <c r="F25" s="4" t="n">
         <v>16906376</v>
@@ -4864,7 +4864,7 @@
         <v>1.50414437019357</v>
       </c>
       <c r="H25" s="3" t="n">
-        <v>-20.2061843395176</v>
+        <v>-25.0672549945982</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4881,7 +4881,7 @@
         <v>24.3737349840969</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>-19.2941365000561</v>
+        <v>-24.2623210556311</v>
       </c>
       <c r="F26" s="4" t="n">
         <v>15959217</v>
@@ -4890,7 +4890,7 @@
         <v>2.92182703718795</v>
       </c>
       <c r="H26" s="3" t="n">
-        <v>-21.9766935928361</v>
+        <v>-27.2881807403761</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4907,7 +4907,7 @@
         <v>8.92721778590047</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>-21.15886313195</v>
+        <v>-26.5625951653375</v>
       </c>
       <c r="F27" s="4" t="n">
         <v>17710222</v>
@@ -4916,7 +4916,7 @@
         <v>6.75570056842025</v>
       </c>
       <c r="H27" s="3" t="n">
-        <v>-23.7845284914514</v>
+        <v>-29.561255677919</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4933,7 +4933,7 @@
         <v>-65.4936014625229</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>-23.0520290149715</v>
+        <v>-28.9032271619792</v>
       </c>
       <c r="F28" s="4" t="n">
         <v>8369465</v>
@@ -4942,7 +4942,7 @@
         <v>-61.1100857519342</v>
       </c>
       <c r="H28" s="3" t="n">
-        <v>-25.6194567308846</v>
+        <v>-31.8741521709843</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4959,7 +4959,7 @@
         <v>-100</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>-24.9604524845686</v>
+        <v>-31.2686970798714</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>0</v>
@@ -4968,7 +4968,7 @@
         <v>-100</v>
       </c>
       <c r="H29" s="3" t="n">
-        <v>-27.4691251574168</v>
+        <v>-34.2120205724792</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4985,7 +4985,7 @@
         <v>-99.2087487938244</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>-26.8738992076092</v>
+        <v>-33.6460259515443</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>259217</v>
@@ -4994,9 +4994,41 @@
         <v>-99.1875549351735</v>
       </c>
       <c r="H30" s="3" t="n">
-        <v>-29.3236452443441</v>
-      </c>
-    </row>
+        <v>-36.5620415084763</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>33324</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>-88.6301136169777</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>-36.0270078166755</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>1820455</v>
+      </c>
+      <c r="G31" s="3" t="n">
+        <v>-95.1014559166552</v>
+      </c>
+      <c r="H31" s="3" t="n">
+        <v>-38.9159642147305</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -23706,13 +23738,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.14"/>
@@ -24505,6 +24537,13 @@
         <v>7.98167030375287</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -25312,7 +25351,7 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J34" activeCellId="0" sqref="J34"/>
     </sheetView>
   </sheetViews>
@@ -26119,7 +26158,7 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -26928,8 +26967,8 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Monthly and quarterly data updates
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_mensual.xlsx
+++ b/etl/data/input/Datos_carga_mensual.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="867" firstSheet="16" activeTab="38"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="867" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Paro" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3220" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3164" uniqueCount="237">
   <si>
     <t/>
   </si>
@@ -8272,8 +8272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -9430,29 +9430,29 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>0</v>
+      <c r="A45" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B45" s="2">
+        <v>8</v>
+      </c>
+      <c r="C45" s="6">
+        <v>673104</v>
+      </c>
+      <c r="D45" s="3">
+        <v>-13.941276873214047</v>
+      </c>
+      <c r="E45" s="3">
+        <v>131.07419408988883</v>
+      </c>
+      <c r="F45" s="6">
+        <v>21649221</v>
+      </c>
+      <c r="G45" s="3">
+        <v>48.105542233558452</v>
+      </c>
+      <c r="H45" s="3">
+        <v>110.02065584132879</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -9700,7 +9700,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -10861,29 +10861,29 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>0</v>
+      <c r="A45" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B45" s="2">
+        <v>8</v>
+      </c>
+      <c r="C45" s="6">
+        <v>128026</v>
+      </c>
+      <c r="D45" s="3">
+        <v>-73.967820186702298</v>
+      </c>
+      <c r="E45" s="3">
+        <v>7.9456020508247178</v>
+      </c>
+      <c r="F45" s="6">
+        <v>17914983</v>
+      </c>
+      <c r="G45" s="3">
+        <v>-0.81150824563600665</v>
+      </c>
+      <c r="H45" s="3">
+        <v>8.939002707055014</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -35480,7 +35480,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD44"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -36596,22 +36596,22 @@
         <v>6</v>
       </c>
       <c r="C43" s="6">
-        <v>101.58</v>
+        <v>101.675</v>
       </c>
       <c r="D43" s="3">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="E43" s="3">
-        <v>4.5246715801993762</v>
+        <v>3.8025777294106282</v>
       </c>
       <c r="F43" s="6">
-        <v>106.10899999999999</v>
+        <v>106.149</v>
       </c>
       <c r="G43" s="3">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="H43" s="3">
-        <v>2.7005945094736958</v>
+        <v>2.3496424086054994</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -36622,48 +36622,48 @@
         <v>7</v>
       </c>
       <c r="C44" s="6">
-        <v>115.779</v>
+        <v>116.34099999999999</v>
       </c>
       <c r="D44" s="3">
-        <v>-1.2</v>
+        <v>-0.7</v>
       </c>
       <c r="E44" s="3">
-        <v>4.9122373661096841</v>
+        <v>4.1367797605947985</v>
       </c>
       <c r="F44" s="6">
-        <v>114.685</v>
+        <v>114.643</v>
       </c>
       <c r="G44" s="3">
         <v>0.1</v>
       </c>
       <c r="H44" s="3">
-        <v>3.0066107279193295</v>
+        <v>2.6297939969878463</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>0</v>
+      <c r="A45" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B45" s="2">
+        <v>8</v>
+      </c>
+      <c r="C45" s="6">
+        <v>115.52</v>
+      </c>
+      <c r="D45" s="3">
+        <v>-2.1</v>
+      </c>
+      <c r="E45" s="3">
+        <v>4.4705255052855462</v>
+      </c>
+      <c r="F45" s="6">
+        <v>102.762</v>
+      </c>
+      <c r="G45" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="H45" s="3">
+        <v>2.9097365758857565</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -36911,7 +36911,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -38027,22 +38027,22 @@
         <v>6</v>
       </c>
       <c r="C43" s="4">
-        <v>101.92700000000001</v>
+        <v>101.97799999999999</v>
       </c>
       <c r="D43" s="3">
         <v>1.9</v>
       </c>
       <c r="E43" s="3">
-        <v>-1.1541038993708475</v>
+        <v>-0.8914130053645718</v>
       </c>
       <c r="F43" s="4">
-        <v>103.73399999999999</v>
+        <v>103.76300000000001</v>
       </c>
       <c r="G43" s="3">
         <v>1.8</v>
       </c>
       <c r="H43" s="3">
-        <v>-1.6253528645168314</v>
+        <v>-1.2546779680139442</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -38053,48 +38053,48 @@
         <v>7</v>
       </c>
       <c r="C44" s="4">
-        <v>104.83499999999999</v>
+        <v>105.01900000000001</v>
       </c>
       <c r="D44" s="3">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="E44" s="3">
-        <v>-1.17653453342547</v>
+        <v>-0.89466136508188898</v>
       </c>
       <c r="F44" s="4">
-        <v>105.047</v>
+        <v>105.089</v>
       </c>
       <c r="G44" s="3">
         <v>2</v>
       </c>
       <c r="H44" s="3">
-        <v>-1.6679428473803912</v>
+        <v>-1.2700570859828151</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>0</v>
+      <c r="A45" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B45" s="2">
+        <v>8</v>
+      </c>
+      <c r="C45" s="4">
+        <v>104.901</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E45" s="3">
+        <v>-0.89777099070262956</v>
+      </c>
+      <c r="F45" s="4">
+        <v>104.545</v>
+      </c>
+      <c r="G45" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="H45" s="3">
+        <v>-1.2852219524272119</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -38342,7 +38342,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -39406,22 +39406,22 @@
         <v>4</v>
       </c>
       <c r="C41" s="4">
-        <v>51</v>
+        <v>433.19600000000003</v>
       </c>
       <c r="D41" s="3">
-        <v>-98.038461538461547</v>
+        <v>25.271032685862348</v>
       </c>
       <c r="E41" s="3">
-        <v>508.08153698302641</v>
+        <v>-6.1751996869182406</v>
       </c>
       <c r="F41" s="4">
-        <v>3468</v>
+        <v>30273.830999999998</v>
       </c>
       <c r="G41" s="3">
-        <v>-98.625467689771071</v>
+        <v>28.56305291944523</v>
       </c>
       <c r="H41" s="3">
-        <v>289.65188471504348</v>
+        <v>-1.186458692923958</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -39432,22 +39432,22 @@
         <v>5</v>
       </c>
       <c r="C42" s="4">
-        <v>0</v>
+        <v>439.32600000000008</v>
       </c>
       <c r="D42" s="3">
-        <v>-100</v>
+        <v>19.165430236879153</v>
       </c>
       <c r="E42" s="3">
-        <v>477.68166669525255</v>
+        <v>-6.6881583913006981</v>
       </c>
       <c r="F42" s="4">
-        <v>3221</v>
+        <v>27048.606</v>
       </c>
       <c r="G42" s="3">
-        <v>-95.474471014696377</v>
+        <v>17.522612103124047</v>
       </c>
       <c r="H42" s="3">
-        <v>277.95593919637673</v>
+        <v>-1.3410943830858328</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -39458,22 +39458,22 @@
         <v>6</v>
       </c>
       <c r="C43" s="4">
-        <v>60</v>
+        <v>407.28699999999998</v>
       </c>
       <c r="D43" s="3">
-        <v>-61.783439490445858</v>
+        <v>17.213662029389255</v>
       </c>
       <c r="E43" s="3">
-        <v>447.1774997630132</v>
+        <v>-7.1946027843935463</v>
       </c>
       <c r="F43" s="4">
-        <v>3605</v>
+        <v>27385.787000000004</v>
       </c>
       <c r="G43" s="3">
-        <v>-88.663165508349323</v>
+        <v>5.4873736763852987</v>
       </c>
       <c r="H43" s="3">
-        <v>266.19191841482825</v>
+        <v>-1.4964967840342147</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -39484,22 +39484,22 @@
         <v>7</v>
       </c>
       <c r="C44" s="4">
-        <v>44</v>
+        <v>416.55199999999996</v>
       </c>
       <c r="D44" s="3">
-        <v>-79.816513761467888</v>
+        <v>27.000271347254355</v>
       </c>
       <c r="E44" s="3">
-        <v>416.63885676337628</v>
+        <v>-7.6986375310365132</v>
       </c>
       <c r="F44" s="4">
-        <v>10217</v>
+        <v>27947.345000000001</v>
       </c>
       <c r="G44" s="3">
-        <v>-58.308169427895209</v>
+        <v>-10.664777928939307</v>
       </c>
       <c r="H44" s="3">
-        <v>254.40618135891958</v>
+        <v>-1.652525035877948</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -41199,7 +41199,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -42334,29 +42334,29 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>0</v>
+      <c r="A44" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B44" s="2">
+        <v>7</v>
+      </c>
+      <c r="C44" s="4">
+        <v>217602.38999999998</v>
+      </c>
+      <c r="D44" s="3">
+        <v>8.1805684876149698</v>
+      </c>
+      <c r="E44" s="3">
+        <v>3.9157596343176819</v>
+      </c>
+      <c r="F44" s="4">
+        <v>15259245.143790001</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0.69042735746940309</v>
+      </c>
+      <c r="H44" s="3">
+        <v>5.0876386087443111</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -42603,7 +42603,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -43725,7 +43725,7 @@
         <v>-37.142857142857146</v>
       </c>
       <c r="E43" s="3">
-        <v>-370.42486139138504</v>
+        <v>-334.09250156954187</v>
       </c>
       <c r="F43" s="4">
         <v>-6387</v>
@@ -43734,33 +43734,33 @@
         <v>17.682691068436654</v>
       </c>
       <c r="H43" s="3">
-        <v>-83.900811523762542</v>
+        <v>-79.237076226313533</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>0</v>
+      <c r="A44" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B44" s="2">
+        <v>7</v>
+      </c>
+      <c r="C44" s="4">
+        <v>37</v>
+      </c>
+      <c r="D44" s="3">
+        <v>-64.423076923076934</v>
+      </c>
+      <c r="E44" s="3">
+        <v>-346.13432516323104</v>
+      </c>
+      <c r="F44" s="4">
+        <v>2471</v>
+      </c>
+      <c r="G44" s="3">
+        <v>-12.870239774330042</v>
+      </c>
+      <c r="H44" s="3">
+        <v>-49.031576349927448</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -46606,8 +46606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -54503,7 +54503,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -55618,14 +55618,14 @@
       <c r="B43" s="2">
         <v>6</v>
       </c>
-      <c r="C43" s="2">
-        <v>-4.3099999999999996</v>
+      <c r="C43" s="3">
+        <v>-4.3139662726818511</v>
       </c>
       <c r="D43" s="3">
-        <v>53.73</v>
+        <v>53.723849450283588</v>
       </c>
       <c r="E43" s="3">
-        <v>11.270354255900644</v>
+        <v>13.67077614112338</v>
       </c>
       <c r="F43" s="2">
         <v>-1.1200000000000001</v>
@@ -55634,7 +55634,7 @@
         <v>21.83</v>
       </c>
       <c r="H43" s="3">
-        <v>5.5138577004078551</v>
+        <v>7.1002958594603758</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -55644,14 +55644,14 @@
       <c r="B44" s="2">
         <v>7</v>
       </c>
-      <c r="C44" s="2">
-        <v>5.21</v>
+      <c r="C44" s="3">
+        <v>5.2057415910831315</v>
       </c>
       <c r="D44" s="3">
-        <v>22.79</v>
+        <v>22.785393630831894</v>
       </c>
       <c r="E44" s="3">
-        <v>15.479011828374633</v>
+        <v>15.102348979845189</v>
       </c>
       <c r="F44" s="2">
         <v>1.02</v>
@@ -55660,7 +55660,7 @@
         <v>14.059999999999999</v>
       </c>
       <c r="H44" s="3">
-        <v>7.6111225872310184</v>
+        <v>7.908380097021924</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -55670,14 +55670,14 @@
       <c r="B45" s="2">
         <v>8</v>
       </c>
-      <c r="C45" s="2">
-        <v>-0.44</v>
+      <c r="C45" s="3">
+        <v>-0.43529048172691515</v>
       </c>
       <c r="D45" s="3">
-        <v>30.15</v>
+        <v>30.159598741432184</v>
       </c>
       <c r="E45" s="3">
-        <v>16.938722468823517</v>
+        <v>16.534432414637077</v>
       </c>
       <c r="F45" s="2">
         <v>1.55</v>
@@ -55686,33 +55686,33 @@
         <v>11.9</v>
       </c>
       <c r="H45" s="3">
-        <v>8.397950126773102</v>
+        <v>8.717029006217567</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>0</v>
+      <c r="A46" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B46" s="2">
+        <v>9</v>
+      </c>
+      <c r="C46" s="3">
+        <v>4.8310046638836432</v>
+      </c>
+      <c r="D46" s="3">
+        <v>14.830006592586022</v>
+      </c>
+      <c r="E46" s="3">
+        <v>17.966298051410991</v>
+      </c>
+      <c r="F46" s="9">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="G46" s="10">
+        <v>12</v>
+      </c>
+      <c r="H46" s="10">
+        <v>9.5258497314040849</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>